<commit_message>
FE-Validation of ROM model done!
</commit_message>
<xml_diff>
--- a/Matlab/Simscape models/Reduced Order Model/summary2ROM.xlsx
+++ b/Matlab/Simscape models/Reduced Order Model/summary2ROM.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28025"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\siril\OneDrive\Desktop\TIM-Control\Matlab\Simscape models\Reduced Order Model\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{675AE67D-F348-4E50-8BA5-77437E508229}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ACD45527-D8FA-42CD-B706-24BA2AEFB49B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -201,18 +201,17 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2323,7 +2322,7 @@
                   </c:numRef>
                 </c:yVal>
                 <c:smooth val="1"/>
-                <c:extLst>
+                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{00000006-837A-4C98-A6A5-F5C7FF181ECC}"/>
                   </c:ext>
@@ -2508,7 +2507,7 @@
                   </c:numRef>
                 </c:yVal>
                 <c:smooth val="1"/>
-                <c:extLst>
+                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{00000001-837A-4C98-A6A5-F5C7FF181ECC}"/>
                   </c:ext>
@@ -2693,7 +2692,7 @@
                   </c:numRef>
                 </c:yVal>
                 <c:smooth val="1"/>
-                <c:extLst>
+                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{00000008-837A-4C98-A6A5-F5C7FF181ECC}"/>
                   </c:ext>
@@ -2878,7 +2877,7 @@
                   </c:numRef>
                 </c:yVal>
                 <c:smooth val="1"/>
-                <c:extLst>
+                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{00000009-837A-4C98-A6A5-F5C7FF181ECC}"/>
                   </c:ext>
@@ -4309,7 +4308,7 @@
                   </c:numRef>
                 </c:yVal>
                 <c:smooth val="1"/>
-                <c:extLst>
+                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{00000006-3E3E-4DFD-8C4F-388186AA14F9}"/>
                   </c:ext>
@@ -4494,7 +4493,7 @@
                   </c:numRef>
                 </c:yVal>
                 <c:smooth val="1"/>
-                <c:extLst>
+                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{00000007-3E3E-4DFD-8C4F-388186AA14F9}"/>
                   </c:ext>
@@ -4679,7 +4678,7 @@
                   </c:numRef>
                 </c:yVal>
                 <c:smooth val="1"/>
-                <c:extLst>
+                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{00000008-3E3E-4DFD-8C4F-388186AA14F9}"/>
                   </c:ext>
@@ -4864,7 +4863,7 @@
                   </c:numRef>
                 </c:yVal>
                 <c:smooth val="1"/>
-                <c:extLst>
+                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{00000009-3E3E-4DFD-8C4F-388186AA14F9}"/>
                   </c:ext>
@@ -9148,7 +9147,7 @@
                   </c:numRef>
                 </c:yVal>
                 <c:smooth val="1"/>
-                <c:extLst>
+                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{00000006-8F52-4599-8E66-84571F941AFE}"/>
                   </c:ext>
@@ -9333,7 +9332,7 @@
                   </c:numRef>
                 </c:yVal>
                 <c:smooth val="1"/>
-                <c:extLst>
+                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{00000007-8F52-4599-8E66-84571F941AFE}"/>
                   </c:ext>
@@ -9518,7 +9517,7 @@
                   </c:numRef>
                 </c:yVal>
                 <c:smooth val="1"/>
-                <c:extLst>
+                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{00000008-8F52-4599-8E66-84571F941AFE}"/>
                   </c:ext>
@@ -9703,7 +9702,7 @@
                   </c:numRef>
                 </c:yVal>
                 <c:smooth val="1"/>
-                <c:extLst>
+                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{00000009-8F52-4599-8E66-84571F941AFE}"/>
                   </c:ext>
@@ -11134,7 +11133,7 @@
                   </c:numRef>
                 </c:yVal>
                 <c:smooth val="1"/>
-                <c:extLst>
+                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{00000006-E516-4879-BEFD-9A248F07B374}"/>
                   </c:ext>
@@ -11319,7 +11318,7 @@
                   </c:numRef>
                 </c:yVal>
                 <c:smooth val="1"/>
-                <c:extLst>
+                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{00000007-E516-4879-BEFD-9A248F07B374}"/>
                   </c:ext>
@@ -11504,7 +11503,7 @@
                   </c:numRef>
                 </c:yVal>
                 <c:smooth val="1"/>
-                <c:extLst>
+                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{00000001-E516-4879-BEFD-9A248F07B374}"/>
                   </c:ext>
@@ -11689,7 +11688,7 @@
                   </c:numRef>
                 </c:yVal>
                 <c:smooth val="1"/>
-                <c:extLst>
+                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{00000009-E516-4879-BEFD-9A248F07B374}"/>
                   </c:ext>
@@ -13120,7 +13119,7 @@
                   </c:numRef>
                 </c:yVal>
                 <c:smooth val="1"/>
-                <c:extLst>
+                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{00000006-DB52-40C8-A5E6-607B16FA5768}"/>
                   </c:ext>
@@ -13305,7 +13304,7 @@
                   </c:numRef>
                 </c:yVal>
                 <c:smooth val="1"/>
-                <c:extLst>
+                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{00000007-DB52-40C8-A5E6-607B16FA5768}"/>
                   </c:ext>
@@ -13490,7 +13489,7 @@
                   </c:numRef>
                 </c:yVal>
                 <c:smooth val="1"/>
-                <c:extLst>
+                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{00000008-DB52-40C8-A5E6-607B16FA5768}"/>
                   </c:ext>
@@ -13675,7 +13674,7 @@
                   </c:numRef>
                 </c:yVal>
                 <c:smooth val="1"/>
-                <c:extLst>
+                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{00000001-DB52-40C8-A5E6-607B16FA5768}"/>
                   </c:ext>
@@ -20494,36 +20493,36 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:W497"/>
+  <dimension ref="A1:V497"/>
   <sheetViews>
     <sheetView topLeftCell="A58" workbookViewId="0">
       <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="13" customWidth="1"/>
-    <col min="7" max="7" width="11.28515625" customWidth="1"/>
-    <col min="8" max="8" width="15.5703125" customWidth="1"/>
+    <col min="7" max="7" width="11.33203125" customWidth="1"/>
+    <col min="8" max="8" width="15.5546875" customWidth="1"/>
     <col min="9" max="9" width="12" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B6" t="s">
         <v>7</v>
       </c>
@@ -20546,7 +20545,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>2</v>
       </c>
@@ -20572,7 +20571,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>3</v>
       </c>
@@ -20598,7 +20597,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>4</v>
       </c>
@@ -20624,7 +20623,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>5</v>
       </c>
@@ -20650,7 +20649,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>6</v>
       </c>
@@ -20676,7 +20675,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>2</v>
       </c>
@@ -20693,7 +20692,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>19</v>
       </c>
@@ -20729,7 +20728,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>18</v>
       </c>
@@ -20761,7 +20760,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="17" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>0</v>
       </c>
@@ -20798,7 +20797,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A18">
         <f>1+A17</f>
         <v>1</v>
@@ -20840,7 +20839,7 @@
         <v>0.70569999999999999</v>
       </c>
     </row>
-    <row r="19" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A19">
         <f t="shared" ref="A19:A26" si="5">1+A18</f>
         <v>2</v>
@@ -20882,7 +20881,7 @@
         <v>1.319</v>
       </c>
     </row>
-    <row r="20" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A20">
         <f t="shared" si="5"/>
         <v>3</v>
@@ -20924,7 +20923,7 @@
         <v>1.9712999999999998</v>
       </c>
     </row>
-    <row r="21" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A21">
         <f t="shared" si="5"/>
         <v>4</v>
@@ -20966,7 +20965,7 @@
         <v>2.7939999999999996</v>
       </c>
     </row>
-    <row r="22" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A22">
         <f t="shared" si="5"/>
         <v>5</v>
@@ -21008,7 +21007,7 @@
         <v>3.9184999999999999</v>
       </c>
     </row>
-    <row r="23" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A23">
         <f t="shared" si="5"/>
         <v>6</v>
@@ -21050,7 +21049,7 @@
         <v>5.4761999999999995</v>
       </c>
     </row>
-    <row r="24" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A24">
         <f t="shared" si="5"/>
         <v>7</v>
@@ -21092,7 +21091,7 @@
         <v>7.5984999999999987</v>
       </c>
     </row>
-    <row r="25" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A25">
         <f t="shared" si="5"/>
         <v>8</v>
@@ -21134,7 +21133,7 @@
         <v>10.416799999999999</v>
       </c>
     </row>
-    <row r="26" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A26">
         <f t="shared" si="5"/>
         <v>9</v>
@@ -21176,7 +21175,7 @@
         <v>14.0625</v>
       </c>
     </row>
-    <row r="27" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A27">
         <f>1+A26</f>
         <v>10</v>
@@ -21218,15 +21217,7 @@
         <v>18.666999999999998</v>
       </c>
     </row>
-    <row r="31" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="R31" s="4"/>
-      <c r="S31" s="4"/>
-      <c r="T31" s="4"/>
-      <c r="U31" s="4"/>
-      <c r="V31" s="4"/>
-      <c r="W31" s="4"/>
-    </row>
-    <row r="32" spans="1:23" ht="60" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:20" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A32" s="2" t="s">
         <v>21</v>
       </c>
@@ -21267,7 +21258,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="33" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>-4.01</v>
       </c>
@@ -21310,7 +21301,7 @@
       <c r="U33" s="3"/>
       <c r="V33" s="3"/>
     </row>
-    <row r="34" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>-3.52</v>
       </c>
@@ -21353,7 +21344,7 @@
       <c r="U34" s="3"/>
       <c r="V34" s="3"/>
     </row>
-    <row r="35" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>-3.02</v>
       </c>
@@ -21396,7 +21387,7 @@
       <c r="U35" s="3"/>
       <c r="V35" s="3"/>
     </row>
-    <row r="36" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>-2.4900000000000002</v>
       </c>
@@ -21439,7 +21430,7 @@
       <c r="U36" s="3"/>
       <c r="V36" s="3"/>
     </row>
-    <row r="37" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A37">
         <v>-2.0099999999999998</v>
       </c>
@@ -21482,7 +21473,7 @@
       <c r="U37" s="3"/>
       <c r="V37" s="3"/>
     </row>
-    <row r="38" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A38">
         <v>-1.5</v>
       </c>
@@ -21525,7 +21516,7 @@
       <c r="U38" s="3"/>
       <c r="V38" s="3"/>
     </row>
-    <row r="39" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A39">
         <v>-0.99</v>
       </c>
@@ -21568,7 +21559,7 @@
       <c r="U39" s="3"/>
       <c r="V39" s="3"/>
     </row>
-    <row r="40" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A40">
         <v>-0.52</v>
       </c>
@@ -21611,7 +21602,7 @@
       <c r="U40" s="3"/>
       <c r="V40" s="3"/>
     </row>
-    <row r="41" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A41">
         <v>0.5</v>
       </c>
@@ -21654,7 +21645,7 @@
       <c r="U41" s="3"/>
       <c r="V41" s="3"/>
     </row>
-    <row r="42" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A42">
         <v>0.98</v>
       </c>
@@ -21697,7 +21688,7 @@
       <c r="U42" s="3"/>
       <c r="V42" s="3"/>
     </row>
-    <row r="43" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A43">
         <v>1.49</v>
       </c>
@@ -21740,7 +21731,7 @@
       <c r="U43" s="3"/>
       <c r="V43" s="3"/>
     </row>
-    <row r="44" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A44">
         <v>2</v>
       </c>
@@ -21783,7 +21774,7 @@
       <c r="U44" s="3"/>
       <c r="V44" s="3"/>
     </row>
-    <row r="45" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A45">
         <v>2.5099999999999998</v>
       </c>
@@ -21826,7 +21817,7 @@
       <c r="U45" s="3"/>
       <c r="V45" s="3"/>
     </row>
-    <row r="46" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A46">
         <v>2.98</v>
       </c>
@@ -21869,7 +21860,7 @@
       <c r="U46" s="3"/>
       <c r="V46" s="3"/>
     </row>
-    <row r="47" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A47">
         <v>3.5</v>
       </c>
@@ -21912,7 +21903,7 @@
       <c r="U47" s="3"/>
       <c r="V47" s="3"/>
     </row>
-    <row r="48" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A48">
         <v>3.99</v>
       </c>
@@ -21955,7 +21946,7 @@
       <c r="U48" s="3"/>
       <c r="V48" s="3"/>
     </row>
-    <row r="49" spans="18:22" x14ac:dyDescent="0.25">
+    <row r="49" spans="18:22" x14ac:dyDescent="0.3">
       <c r="R49">
         <v>4.7237631482134406E-6</v>
       </c>
@@ -21968,7 +21959,7 @@
       <c r="U49" s="3"/>
       <c r="V49" s="3"/>
     </row>
-    <row r="50" spans="18:22" x14ac:dyDescent="0.25">
+    <row r="50" spans="18:22" x14ac:dyDescent="0.3">
       <c r="R50">
         <v>5.3650568239869995E-6</v>
       </c>
@@ -21980,7 +21971,7 @@
       </c>
       <c r="U50" s="3"/>
     </row>
-    <row r="51" spans="18:22" x14ac:dyDescent="0.25">
+    <row r="51" spans="18:22" x14ac:dyDescent="0.3">
       <c r="R51">
         <v>6.0063504997605584E-6</v>
       </c>
@@ -21992,7 +21983,7 @@
       </c>
       <c r="U51" s="3"/>
     </row>
-    <row r="52" spans="18:22" x14ac:dyDescent="0.25">
+    <row r="52" spans="18:22" x14ac:dyDescent="0.3">
       <c r="R52">
         <v>7.4316213781017053E-6</v>
       </c>
@@ -22004,7 +21995,7 @@
       </c>
       <c r="U52" s="3"/>
     </row>
-    <row r="53" spans="18:22" x14ac:dyDescent="0.25">
+    <row r="53" spans="18:22" x14ac:dyDescent="0.3">
       <c r="R53">
         <v>8.8568922564428531E-6</v>
       </c>
@@ -22016,7 +22007,7 @@
       </c>
       <c r="U53" s="3"/>
     </row>
-    <row r="54" spans="18:22" x14ac:dyDescent="0.25">
+    <row r="54" spans="18:22" x14ac:dyDescent="0.3">
       <c r="R54">
         <v>1.0282163134784001E-5</v>
       </c>
@@ -22028,7 +22019,7 @@
       </c>
       <c r="U54" s="3"/>
     </row>
-    <row r="55" spans="18:22" x14ac:dyDescent="0.25">
+    <row r="55" spans="18:22" x14ac:dyDescent="0.3">
       <c r="R55">
         <v>1.1707434013125149E-5</v>
       </c>
@@ -22040,7 +22031,7 @@
       </c>
       <c r="U55" s="3"/>
     </row>
-    <row r="56" spans="18:22" x14ac:dyDescent="0.25">
+    <row r="56" spans="18:22" x14ac:dyDescent="0.3">
       <c r="R56">
         <v>1.3132704891466296E-5</v>
       </c>
@@ -22052,7 +22043,7 @@
       </c>
       <c r="U56" s="3"/>
     </row>
-    <row r="57" spans="18:22" x14ac:dyDescent="0.25">
+    <row r="57" spans="18:22" x14ac:dyDescent="0.3">
       <c r="R57">
         <v>1.5452113221328384E-5</v>
       </c>
@@ -22064,7 +22055,7 @@
       </c>
       <c r="U57" s="3"/>
     </row>
-    <row r="58" spans="18:22" x14ac:dyDescent="0.25">
+    <row r="58" spans="18:22" x14ac:dyDescent="0.3">
       <c r="R58">
         <v>1.777152155119047E-5</v>
       </c>
@@ -22076,7 +22067,7 @@
       </c>
       <c r="U58" s="3"/>
     </row>
-    <row r="59" spans="18:22" x14ac:dyDescent="0.25">
+    <row r="59" spans="18:22" x14ac:dyDescent="0.3">
       <c r="R59">
         <v>2.0090929881052556E-5</v>
       </c>
@@ -22088,7 +22079,7 @@
       </c>
       <c r="U59" s="3"/>
     </row>
-    <row r="60" spans="18:22" x14ac:dyDescent="0.25">
+    <row r="60" spans="18:22" x14ac:dyDescent="0.3">
       <c r="R60">
         <v>2.2410338210914641E-5</v>
       </c>
@@ -22100,7 +22091,7 @@
       </c>
       <c r="U60" s="3"/>
     </row>
-    <row r="61" spans="18:22" x14ac:dyDescent="0.25">
+    <row r="61" spans="18:22" x14ac:dyDescent="0.3">
       <c r="R61">
         <v>2.4729746540776727E-5</v>
       </c>
@@ -22112,7 +22103,7 @@
       </c>
       <c r="U61" s="3"/>
     </row>
-    <row r="62" spans="18:22" x14ac:dyDescent="0.25">
+    <row r="62" spans="18:22" x14ac:dyDescent="0.3">
       <c r="R62">
         <v>2.8469147114721976E-5</v>
       </c>
@@ -22124,7 +22115,7 @@
       </c>
       <c r="U62" s="3"/>
     </row>
-    <row r="63" spans="18:22" x14ac:dyDescent="0.25">
+    <row r="63" spans="18:22" x14ac:dyDescent="0.3">
       <c r="R63">
         <v>3.2208547688667226E-5</v>
       </c>
@@ -22136,7 +22127,7 @@
       </c>
       <c r="U63" s="3"/>
     </row>
-    <row r="64" spans="18:22" x14ac:dyDescent="0.25">
+    <row r="64" spans="18:22" x14ac:dyDescent="0.3">
       <c r="R64">
         <v>3.5947948262612475E-5</v>
       </c>
@@ -22148,7 +22139,7 @@
       </c>
       <c r="U64" s="3"/>
     </row>
-    <row r="65" spans="18:21" x14ac:dyDescent="0.25">
+    <row r="65" spans="18:21" x14ac:dyDescent="0.3">
       <c r="R65">
         <v>3.9687348836557725E-5</v>
       </c>
@@ -22160,7 +22151,7 @@
       </c>
       <c r="U65" s="3"/>
     </row>
-    <row r="66" spans="18:21" x14ac:dyDescent="0.25">
+    <row r="66" spans="18:21" x14ac:dyDescent="0.3">
       <c r="R66">
         <v>4.3426749410502974E-5</v>
       </c>
@@ -22172,7 +22163,7 @@
       </c>
       <c r="U66" s="3"/>
     </row>
-    <row r="67" spans="18:21" x14ac:dyDescent="0.25">
+    <row r="67" spans="18:21" x14ac:dyDescent="0.3">
       <c r="R67">
         <v>5.1106793548755923E-5</v>
       </c>
@@ -22184,7 +22175,7 @@
       </c>
       <c r="U67" s="3"/>
     </row>
-    <row r="68" spans="18:21" x14ac:dyDescent="0.25">
+    <row r="68" spans="18:21" x14ac:dyDescent="0.3">
       <c r="R68">
         <v>5.8786837687008873E-5</v>
       </c>
@@ -22196,7 +22187,7 @@
       </c>
       <c r="U68" s="3"/>
     </row>
-    <row r="69" spans="18:21" x14ac:dyDescent="0.25">
+    <row r="69" spans="18:21" x14ac:dyDescent="0.3">
       <c r="R69">
         <v>6.6466881825261829E-5</v>
       </c>
@@ -22208,7 +22199,7 @@
       </c>
       <c r="U69" s="3"/>
     </row>
-    <row r="70" spans="18:21" x14ac:dyDescent="0.25">
+    <row r="70" spans="18:21" x14ac:dyDescent="0.3">
       <c r="R70">
         <v>7.4146925963514785E-5</v>
       </c>
@@ -22220,7 +22211,7 @@
       </c>
       <c r="U70" s="3"/>
     </row>
-    <row r="71" spans="18:21" x14ac:dyDescent="0.25">
+    <row r="71" spans="18:21" x14ac:dyDescent="0.3">
       <c r="R71">
         <v>8.1826970101767741E-5</v>
       </c>
@@ -22231,7 +22222,7 @@
         <v>-2.0855509848871634E-5</v>
       </c>
     </row>
-    <row r="72" spans="18:21" x14ac:dyDescent="0.25">
+    <row r="72" spans="18:21" x14ac:dyDescent="0.3">
       <c r="R72">
         <v>9.2761152528282405E-5</v>
       </c>
@@ -22242,7 +22233,7 @@
         <v>-1.9893205557508509E-5</v>
       </c>
     </row>
-    <row r="73" spans="18:21" x14ac:dyDescent="0.25">
+    <row r="73" spans="18:21" x14ac:dyDescent="0.3">
       <c r="R73">
         <v>1.0369533495479707E-4</v>
       </c>
@@ -22253,7 +22244,7 @@
         <v>-1.9008731589664762E-5</v>
       </c>
     </row>
-    <row r="74" spans="18:21" x14ac:dyDescent="0.25">
+    <row r="74" spans="18:21" x14ac:dyDescent="0.3">
       <c r="R74">
         <v>1.1462951738131173E-4</v>
       </c>
@@ -22264,7 +22255,7 @@
         <v>-1.8211242785781678E-5</v>
       </c>
     </row>
-    <row r="75" spans="18:21" x14ac:dyDescent="0.25">
+    <row r="75" spans="18:21" x14ac:dyDescent="0.3">
       <c r="R75">
         <v>1.2556369980782641E-4</v>
       </c>
@@ -22275,7 +22266,7 @@
         <v>-1.7505849236876259E-5</v>
       </c>
     </row>
-    <row r="76" spans="18:21" x14ac:dyDescent="0.25">
+    <row r="76" spans="18:21" x14ac:dyDescent="0.3">
       <c r="R76">
         <v>1.3649788223434107E-4</v>
       </c>
@@ -22286,7 +22277,7 @@
         <v>-1.6894769417241662E-5</v>
       </c>
     </row>
-    <row r="77" spans="18:21" x14ac:dyDescent="0.25">
+    <row r="77" spans="18:21" x14ac:dyDescent="0.3">
       <c r="R77">
         <v>1.4743206466085574E-4</v>
       </c>
@@ -22297,7 +22288,7 @@
         <v>-1.6378085009094434E-5</v>
       </c>
     </row>
-    <row r="78" spans="18:21" x14ac:dyDescent="0.25">
+    <row r="78" spans="18:21" x14ac:dyDescent="0.3">
       <c r="R78">
         <v>1.6595040333127164E-4</v>
       </c>
@@ -22308,7 +22299,7 @@
         <v>-1.5714419318690886E-5</v>
       </c>
     </row>
-    <row r="79" spans="18:21" x14ac:dyDescent="0.25">
+    <row r="79" spans="18:21" x14ac:dyDescent="0.3">
       <c r="R79">
         <v>1.8446874200168755E-4</v>
       </c>
@@ -22319,7 +22310,7 @@
         <v>-1.5305147671895725E-5</v>
       </c>
     </row>
-    <row r="80" spans="18:21" x14ac:dyDescent="0.25">
+    <row r="80" spans="18:21" x14ac:dyDescent="0.3">
       <c r="R80">
         <v>2.0298708067210345E-4</v>
       </c>
@@ -22330,7 +22321,7 @@
         <v>-1.5134383099635329E-5</v>
       </c>
     </row>
-    <row r="81" spans="18:20" x14ac:dyDescent="0.25">
+    <row r="81" spans="18:20" x14ac:dyDescent="0.3">
       <c r="R81">
         <v>2.2150541934251936E-4</v>
       </c>
@@ -22341,7 +22332,7 @@
         <v>-1.5185534228301378E-5</v>
       </c>
     </row>
-    <row r="82" spans="18:20" x14ac:dyDescent="0.25">
+    <row r="82" spans="18:20" x14ac:dyDescent="0.3">
       <c r="R82">
         <v>2.4002375801293526E-4</v>
       </c>
@@ -22352,7 +22343,7 @@
         <v>-1.5441990675491013E-5</v>
       </c>
     </row>
-    <row r="83" spans="18:20" x14ac:dyDescent="0.25">
+    <row r="83" spans="18:20" x14ac:dyDescent="0.3">
       <c r="R83">
         <v>2.5854209668335116E-4</v>
       </c>
@@ -22363,7 +22354,7 @@
         <v>-1.5887338638442827E-5</v>
       </c>
     </row>
-    <row r="84" spans="18:20" x14ac:dyDescent="0.25">
+    <row r="84" spans="18:20" x14ac:dyDescent="0.3">
       <c r="R84">
         <v>2.9600453495756636E-4</v>
       </c>
@@ -22374,7 +22365,7 @@
         <v>-1.7302456208234673E-5</v>
       </c>
     </row>
-    <row r="85" spans="18:20" x14ac:dyDescent="0.25">
+    <row r="85" spans="18:20" x14ac:dyDescent="0.3">
       <c r="R85">
         <v>3.3346697323178155E-4</v>
       </c>
@@ -22385,7 +22376,7 @@
         <v>-1.9307870998019894E-5</v>
       </c>
     </row>
-    <row r="86" spans="18:20" x14ac:dyDescent="0.25">
+    <row r="86" spans="18:20" x14ac:dyDescent="0.3">
       <c r="R86">
         <v>3.7092941150599674E-4</v>
       </c>
@@ -22396,7 +22387,7 @@
         <v>-2.1800689309792176E-5</v>
       </c>
     </row>
-    <row r="87" spans="18:20" x14ac:dyDescent="0.25">
+    <row r="87" spans="18:20" x14ac:dyDescent="0.3">
       <c r="R87">
         <v>4.0839184978021194E-4</v>
       </c>
@@ -22407,7 +22398,7 @@
         <v>-2.4693176849943654E-5</v>
       </c>
     </row>
-    <row r="88" spans="18:20" x14ac:dyDescent="0.25">
+    <row r="88" spans="18:20" x14ac:dyDescent="0.3">
       <c r="R88">
         <v>4.4585428805442713E-4</v>
       </c>
@@ -22418,7 +22409,7 @@
         <v>-2.7909535623926729E-5</v>
       </c>
     </row>
-    <row r="89" spans="18:20" x14ac:dyDescent="0.25">
+    <row r="89" spans="18:20" x14ac:dyDescent="0.3">
       <c r="R89">
         <v>4.8331672632864232E-4</v>
       </c>
@@ -22429,7 +22420,7 @@
         <v>-3.1384029388625834E-5</v>
       </c>
     </row>
-    <row r="90" spans="18:20" x14ac:dyDescent="0.25">
+    <row r="90" spans="18:20" x14ac:dyDescent="0.3">
       <c r="R90">
         <v>5.5903858519549383E-4</v>
       </c>
@@ -22440,7 +22431,7 @@
         <v>-3.898384986555925E-5</v>
       </c>
     </row>
-    <row r="91" spans="18:20" x14ac:dyDescent="0.25">
+    <row r="91" spans="18:20" x14ac:dyDescent="0.3">
       <c r="R91">
         <v>6.3476044406234533E-4</v>
       </c>
@@ -22451,7 +22442,7 @@
         <v>-4.7043714715755414E-5</v>
       </c>
     </row>
-    <row r="92" spans="18:20" x14ac:dyDescent="0.25">
+    <row r="92" spans="18:20" x14ac:dyDescent="0.3">
       <c r="R92">
         <v>7.1048230292919683E-4</v>
       </c>
@@ -22462,7 +22453,7 @@
         <v>-5.5284955912782152E-5</v>
       </c>
     </row>
-    <row r="93" spans="18:20" x14ac:dyDescent="0.25">
+    <row r="93" spans="18:20" x14ac:dyDescent="0.3">
       <c r="R93">
         <v>7.8620416179604833E-4</v>
       </c>
@@ -22473,7 +22464,7 @@
         <v>-6.3509565030095416E-5</v>
       </c>
     </row>
-    <row r="94" spans="18:20" x14ac:dyDescent="0.25">
+    <row r="94" spans="18:20" x14ac:dyDescent="0.3">
       <c r="R94">
         <v>8.6192602066289983E-4</v>
       </c>
@@ -22484,7 +22475,7 @@
         <v>-7.1573746994069154E-5</v>
       </c>
     </row>
-    <row r="95" spans="18:20" x14ac:dyDescent="0.25">
+    <row r="95" spans="18:20" x14ac:dyDescent="0.3">
       <c r="R95">
         <v>9.5660142301658114E-4</v>
       </c>
@@ -22495,7 +22486,7 @@
         <v>-8.127400577606636E-5</v>
       </c>
     </row>
-    <row r="96" spans="18:20" x14ac:dyDescent="0.25">
+    <row r="96" spans="18:20" x14ac:dyDescent="0.3">
       <c r="R96">
         <v>1.0512768253702624E-3</v>
       </c>
@@ -22506,7 +22497,7 @@
         <v>-9.0404810446642614E-5</v>
       </c>
     </row>
-    <row r="97" spans="18:20" x14ac:dyDescent="0.25">
+    <row r="97" spans="18:20" x14ac:dyDescent="0.3">
       <c r="R97">
         <v>1.1459522277239439E-3</v>
       </c>
@@ -22517,7 +22508,7 @@
         <v>-9.8861075207956617E-5</v>
       </c>
     </row>
-    <row r="98" spans="18:20" x14ac:dyDescent="0.25">
+    <row r="98" spans="18:20" x14ac:dyDescent="0.3">
       <c r="R98">
         <v>1.2406276300776253E-3</v>
       </c>
@@ -22528,7 +22519,7 @@
         <v>-1.0657270926017759E-4</v>
       </c>
     </row>
-    <row r="99" spans="18:20" x14ac:dyDescent="0.25">
+    <row r="99" spans="18:20" x14ac:dyDescent="0.3">
       <c r="R99">
         <v>1.3353030324313067E-3</v>
       </c>
@@ -22539,7 +22530,7 @@
         <v>-1.1349151243589262E-4</v>
       </c>
     </row>
-    <row r="100" spans="18:20" x14ac:dyDescent="0.25">
+    <row r="100" spans="18:20" x14ac:dyDescent="0.3">
       <c r="R100">
         <v>1.4830986028998225E-3</v>
       </c>
@@ -22550,7 +22541,7 @@
         <v>-1.226337235076258E-4</v>
       </c>
     </row>
-    <row r="101" spans="18:20" x14ac:dyDescent="0.25">
+    <row r="101" spans="18:20" x14ac:dyDescent="0.3">
       <c r="R101">
         <v>1.6308941733683383E-3</v>
       </c>
@@ -22561,7 +22552,7 @@
         <v>-1.2967428406884807E-4</v>
       </c>
     </row>
-    <row r="102" spans="18:20" x14ac:dyDescent="0.25">
+    <row r="102" spans="18:20" x14ac:dyDescent="0.3">
       <c r="R102">
         <v>1.7786897438368541E-3</v>
       </c>
@@ -22572,7 +22563,7 @@
         <v>-1.3456056319416376E-4</v>
       </c>
     </row>
-    <row r="103" spans="18:20" x14ac:dyDescent="0.25">
+    <row r="103" spans="18:20" x14ac:dyDescent="0.3">
       <c r="R103">
         <v>1.9264853143053698E-3</v>
       </c>
@@ -22583,7 +22574,7 @@
         <v>-1.3726221722976106E-4</v>
       </c>
     </row>
-    <row r="104" spans="18:20" x14ac:dyDescent="0.25">
+    <row r="104" spans="18:20" x14ac:dyDescent="0.3">
       <c r="R104">
         <v>2.0742808847738856E-3</v>
       </c>
@@ -22594,7 +22585,7 @@
         <v>-1.3775834886065041E-4</v>
       </c>
     </row>
-    <row r="105" spans="18:20" x14ac:dyDescent="0.25">
+    <row r="105" spans="18:20" x14ac:dyDescent="0.3">
       <c r="R105">
         <v>2.3598784316873475E-3</v>
       </c>
@@ -22605,7 +22596,7 @@
         <v>-1.3241058341151302E-4</v>
       </c>
     </row>
-    <row r="106" spans="18:20" x14ac:dyDescent="0.25">
+    <row r="106" spans="18:20" x14ac:dyDescent="0.3">
       <c r="R106">
         <v>2.6454759786008093E-3</v>
       </c>
@@ -22616,7 +22607,7 @@
         <v>-1.1866903903179349E-4</v>
       </c>
     </row>
-    <row r="107" spans="18:20" x14ac:dyDescent="0.25">
+    <row r="107" spans="18:20" x14ac:dyDescent="0.3">
       <c r="R107">
         <v>2.9310735255142712E-3</v>
       </c>
@@ -22627,7 +22618,7 @@
         <v>-9.64578993434273E-5</v>
       </c>
     </row>
-    <row r="108" spans="18:20" x14ac:dyDescent="0.25">
+    <row r="108" spans="18:20" x14ac:dyDescent="0.3">
       <c r="R108">
         <v>3.216671072427733E-3</v>
       </c>
@@ -22638,7 +22629,7 @@
         <v>-6.5711275371249656E-5</v>
       </c>
     </row>
-    <row r="109" spans="18:20" x14ac:dyDescent="0.25">
+    <row r="109" spans="18:20" x14ac:dyDescent="0.3">
       <c r="R109">
         <v>3.5022686193411949E-3</v>
       </c>
@@ -22649,7 +22640,7 @@
         <v>-2.6365157554941732E-5</v>
       </c>
     </row>
-    <row r="110" spans="18:20" x14ac:dyDescent="0.25">
+    <row r="110" spans="18:20" x14ac:dyDescent="0.3">
       <c r="R110">
         <v>5.0964253405883855E-3</v>
       </c>
@@ -22660,7 +22651,7 @@
         <v>3.5390029556747749E-4</v>
       </c>
     </row>
-    <row r="111" spans="18:20" x14ac:dyDescent="0.25">
+    <row r="111" spans="18:20" x14ac:dyDescent="0.3">
       <c r="R111">
         <v>6.6905820618355771E-3</v>
       </c>
@@ -22671,7 +22662,7 @@
         <v>1.0134605714098299E-3</v>
       </c>
     </row>
-    <row r="112" spans="18:20" x14ac:dyDescent="0.25">
+    <row r="112" spans="18:20" x14ac:dyDescent="0.3">
       <c r="R112">
         <v>8.2847387830827686E-3</v>
       </c>
@@ -22682,7 +22673,7 @@
         <v>1.9602013585648947E-3</v>
       </c>
     </row>
-    <row r="113" spans="18:20" x14ac:dyDescent="0.25">
+    <row r="113" spans="18:20" x14ac:dyDescent="0.3">
       <c r="R113">
         <v>9.8788955043299601E-3</v>
       </c>
@@ -22693,7 +22684,7 @@
         <v>3.2001187388264185E-3</v>
       </c>
     </row>
-    <row r="114" spans="18:20" x14ac:dyDescent="0.25">
+    <row r="114" spans="18:20" x14ac:dyDescent="0.3">
       <c r="R114">
         <v>1.1473052225577152E-2</v>
       </c>
@@ -22704,7 +22695,7 @@
         <v>4.7374399637494236E-3</v>
       </c>
     </row>
-    <row r="115" spans="18:20" x14ac:dyDescent="0.25">
+    <row r="115" spans="18:20" x14ac:dyDescent="0.3">
       <c r="R115">
         <v>1.4216075616809778E-2</v>
       </c>
@@ -22715,7 +22706,7 @@
         <v>8.0844827911716877E-3</v>
       </c>
     </row>
-    <row r="116" spans="18:20" x14ac:dyDescent="0.25">
+    <row r="116" spans="18:20" x14ac:dyDescent="0.3">
       <c r="R116">
         <v>1.6959099008042405E-2</v>
       </c>
@@ -22726,7 +22717,7 @@
         <v>1.2321948613661426E-2</v>
       </c>
     </row>
-    <row r="117" spans="18:20" x14ac:dyDescent="0.25">
+    <row r="117" spans="18:20" x14ac:dyDescent="0.3">
       <c r="R117">
         <v>1.9702122399275032E-2</v>
       </c>
@@ -22737,7 +22728,7 @@
         <v>1.7441594139151917E-2</v>
       </c>
     </row>
-    <row r="118" spans="18:20" x14ac:dyDescent="0.25">
+    <row r="118" spans="18:20" x14ac:dyDescent="0.3">
       <c r="R118">
         <v>0.02</v>
       </c>
@@ -22748,7 +22739,7 @@
         <v>1.8050142377103562E-2</v>
       </c>
     </row>
-    <row r="119" spans="18:20" x14ac:dyDescent="0.25">
+    <row r="119" spans="18:20" x14ac:dyDescent="0.3">
       <c r="R119">
         <v>2.0297877600724969E-2</v>
       </c>
@@ -22759,7 +22750,7 @@
         <v>1.8668766756588795E-2</v>
       </c>
     </row>
-    <row r="120" spans="18:20" x14ac:dyDescent="0.25">
+    <row r="120" spans="18:20" x14ac:dyDescent="0.3">
       <c r="R120">
         <v>2.0595755201449937E-2</v>
       </c>
@@ -22770,7 +22761,7 @@
         <v>1.9297473347556604E-2</v>
       </c>
     </row>
-    <row r="121" spans="18:20" x14ac:dyDescent="0.25">
+    <row r="121" spans="18:20" x14ac:dyDescent="0.3">
       <c r="R121">
         <v>2.0893632802174905E-2</v>
       </c>
@@ -22781,7 +22772,7 @@
         <v>1.9936259566103232E-2</v>
       </c>
     </row>
-    <row r="122" spans="18:20" x14ac:dyDescent="0.25">
+    <row r="122" spans="18:20" x14ac:dyDescent="0.3">
       <c r="R122">
         <v>2.1191510402899873E-2</v>
       </c>
@@ -22792,7 +22783,7 @@
         <v>2.0585098486575859E-2</v>
       </c>
     </row>
-    <row r="123" spans="18:20" x14ac:dyDescent="0.25">
+    <row r="123" spans="18:20" x14ac:dyDescent="0.3">
       <c r="R123">
         <v>2.2766680724121222E-2</v>
       </c>
@@ -22803,7 +22794,7 @@
         <v>2.4180751569994996E-2</v>
       </c>
     </row>
-    <row r="124" spans="18:20" x14ac:dyDescent="0.25">
+    <row r="124" spans="18:20" x14ac:dyDescent="0.3">
       <c r="R124">
         <v>2.4341851045342571E-2</v>
       </c>
@@ -22814,7 +22805,7 @@
         <v>2.8050022722740486E-2</v>
       </c>
     </row>
-    <row r="125" spans="18:20" x14ac:dyDescent="0.25">
+    <row r="125" spans="18:20" x14ac:dyDescent="0.3">
       <c r="R125">
         <v>2.591702136656392E-2</v>
       </c>
@@ -22825,7 +22816,7 @@
         <v>3.2186525197572813E-2</v>
       </c>
     </row>
-    <row r="126" spans="18:20" x14ac:dyDescent="0.25">
+    <row r="126" spans="18:20" x14ac:dyDescent="0.3">
       <c r="R126">
         <v>2.7492191687785269E-2</v>
       </c>
@@ -22836,7 +22827,7 @@
         <v>3.6583010822416995E-2</v>
       </c>
     </row>
-    <row r="127" spans="18:20" x14ac:dyDescent="0.25">
+    <row r="127" spans="18:20" x14ac:dyDescent="0.3">
       <c r="R127">
         <v>3.0018237840883633E-2</v>
       </c>
@@ -22847,7 +22838,7 @@
         <v>4.4157256933597289E-2</v>
       </c>
     </row>
-    <row r="128" spans="18:20" x14ac:dyDescent="0.25">
+    <row r="128" spans="18:20" x14ac:dyDescent="0.3">
       <c r="R128">
         <v>3.2544283993982001E-2</v>
       </c>
@@ -22858,7 +22849,7 @@
         <v>5.2345675359352306E-2</v>
       </c>
     </row>
-    <row r="129" spans="18:20" x14ac:dyDescent="0.25">
+    <row r="129" spans="18:20" x14ac:dyDescent="0.3">
       <c r="R129">
         <v>3.5070330147080366E-2</v>
       </c>
@@ -22869,7 +22860,7 @@
         <v>6.1109951164411314E-2</v>
       </c>
     </row>
-    <row r="130" spans="18:20" x14ac:dyDescent="0.25">
+    <row r="130" spans="18:20" x14ac:dyDescent="0.3">
       <c r="R130">
         <v>3.759637630017873E-2</v>
       </c>
@@ -22880,7 +22871,7 @@
         <v>7.0409850577108024E-2</v>
       </c>
     </row>
-    <row r="131" spans="18:20" x14ac:dyDescent="0.25">
+    <row r="131" spans="18:20" x14ac:dyDescent="0.3">
       <c r="R131">
         <v>0.04</v>
       </c>
@@ -22891,7 +22882,7 @@
         <v>7.9718709366076723E-2</v>
       </c>
     </row>
-    <row r="132" spans="18:20" x14ac:dyDescent="0.25">
+    <row r="132" spans="18:20" x14ac:dyDescent="0.3">
       <c r="R132">
         <v>4.2403623699821272E-2</v>
       </c>
@@ -22902,7 +22893,7 @@
         <v>8.9439307013387648E-2</v>
       </c>
     </row>
-    <row r="133" spans="18:20" x14ac:dyDescent="0.25">
+    <row r="133" spans="18:20" x14ac:dyDescent="0.3">
       <c r="R133">
         <v>4.4807247399642543E-2</v>
       </c>
@@ -22913,7 +22904,7 @@
         <v>9.9535764372688185E-2</v>
       </c>
     </row>
-    <row r="134" spans="18:20" x14ac:dyDescent="0.25">
+    <row r="134" spans="18:20" x14ac:dyDescent="0.3">
       <c r="R134">
         <v>4.7210871099463814E-2</v>
       </c>
@@ -22924,7 +22915,7 @@
         <v>0.10997257318813425</v>
       </c>
     </row>
-    <row r="135" spans="18:20" x14ac:dyDescent="0.25">
+    <row r="135" spans="18:20" x14ac:dyDescent="0.3">
       <c r="R135">
         <v>4.9614494799285085E-2</v>
       </c>
@@ -22935,7 +22926,7 @@
         <v>0.120714929490644</v>
       </c>
     </row>
-    <row r="136" spans="18:20" x14ac:dyDescent="0.25">
+    <row r="136" spans="18:20" x14ac:dyDescent="0.3">
       <c r="R136">
         <v>5.4257973747477116E-2</v>
       </c>
@@ -22946,7 +22937,7 @@
         <v>0.14221031259089312</v>
       </c>
     </row>
-    <row r="137" spans="18:20" x14ac:dyDescent="0.25">
+    <row r="137" spans="18:20" x14ac:dyDescent="0.3">
       <c r="R137">
         <v>5.8901452695669147E-2</v>
       </c>
@@ -22957,7 +22948,7 @@
         <v>0.1644929163358384</v>
       </c>
     </row>
-    <row r="138" spans="18:20" x14ac:dyDescent="0.25">
+    <row r="138" spans="18:20" x14ac:dyDescent="0.3">
       <c r="R138">
         <v>0.06</v>
       </c>
@@ -22968,7 +22959,7 @@
         <v>0.16985551136455967</v>
       </c>
     </row>
-    <row r="139" spans="18:20" x14ac:dyDescent="0.25">
+    <row r="139" spans="18:20" x14ac:dyDescent="0.3">
       <c r="R139">
         <v>6.1098547304330848E-2</v>
       </c>
@@ -22979,7 +22970,7 @@
         <v>0.17524793179803311</v>
       </c>
     </row>
-    <row r="140" spans="18:20" x14ac:dyDescent="0.25">
+    <row r="140" spans="18:20" x14ac:dyDescent="0.3">
       <c r="R140">
         <v>6.2197094608661699E-2</v>
       </c>
@@ -22990,7 +22981,7 @@
         <v>0.1806677113185744</v>
       </c>
     </row>
-    <row r="141" spans="18:20" x14ac:dyDescent="0.25">
+    <row r="141" spans="18:20" x14ac:dyDescent="0.3">
       <c r="R141">
         <v>6.3295641912992556E-2</v>
       </c>
@@ -23001,7 +22992,7 @@
         <v>0.18611240566419696</v>
       </c>
     </row>
-    <row r="142" spans="18:20" x14ac:dyDescent="0.25">
+    <row r="142" spans="18:20" x14ac:dyDescent="0.3">
       <c r="R142">
         <v>6.43941892173234E-2</v>
       </c>
@@ -23012,7 +23003,7 @@
         <v>0.19157968896710109</v>
       </c>
     </row>
-    <row r="143" spans="18:20" x14ac:dyDescent="0.25">
+    <row r="143" spans="18:20" x14ac:dyDescent="0.3">
       <c r="R143">
         <v>6.9375854916671698E-2</v>
       </c>
@@ -23023,7 +23014,7 @@
         <v>0.21660057753826312</v>
       </c>
     </row>
-    <row r="144" spans="18:20" x14ac:dyDescent="0.25">
+    <row r="144" spans="18:20" x14ac:dyDescent="0.3">
       <c r="R144">
         <v>7.4357520616019995E-2</v>
       </c>
@@ -23034,7 +23025,7 @@
         <v>0.24186122998287019</v>
       </c>
     </row>
-    <row r="145" spans="18:20" x14ac:dyDescent="0.25">
+    <row r="145" spans="18:20" x14ac:dyDescent="0.3">
       <c r="R145">
         <v>7.9339186315368293E-2</v>
       </c>
@@ -23045,7 +23036,7 @@
         <v>0.26721018827739229</v>
       </c>
     </row>
-    <row r="146" spans="18:20" x14ac:dyDescent="0.25">
+    <row r="146" spans="18:20" x14ac:dyDescent="0.3">
       <c r="R146">
         <v>0.08</v>
       </c>
@@ -23056,7 +23047,7 @@
         <v>0.27057191888932053</v>
       </c>
     </row>
-    <row r="147" spans="18:20" x14ac:dyDescent="0.25">
+    <row r="147" spans="18:20" x14ac:dyDescent="0.3">
       <c r="R147">
         <v>8.066081368463171E-2</v>
       </c>
@@ -23067,7 +23058,7 @@
         <v>0.27393312401634606</v>
       </c>
     </row>
-    <row r="148" spans="18:20" x14ac:dyDescent="0.25">
+    <row r="148" spans="18:20" x14ac:dyDescent="0.3">
       <c r="R148">
         <v>8.1321627369263419E-2</v>
       </c>
@@ -23078,7 +23069,7 @@
         <v>0.27729347731777221</v>
       </c>
     </row>
-    <row r="149" spans="18:20" x14ac:dyDescent="0.25">
+    <row r="149" spans="18:20" x14ac:dyDescent="0.3">
       <c r="R149">
         <v>8.1982441053895128E-2</v>
       </c>
@@ -23089,7 +23080,7 @@
         <v>0.28065266511952913</v>
       </c>
     </row>
-    <row r="150" spans="18:20" x14ac:dyDescent="0.25">
+    <row r="150" spans="18:20" x14ac:dyDescent="0.3">
       <c r="R150">
         <v>8.2643254738526836E-2</v>
       </c>
@@ -23100,7 +23091,7 @@
         <v>0.28401045562531113</v>
       </c>
     </row>
-    <row r="151" spans="18:20" x14ac:dyDescent="0.25">
+    <row r="151" spans="18:20" x14ac:dyDescent="0.3">
       <c r="R151">
         <v>8.6527040595524046E-2</v>
       </c>
@@ -23111,7 +23102,7 @@
         <v>0.30370344348290779</v>
       </c>
     </row>
-    <row r="152" spans="18:20" x14ac:dyDescent="0.25">
+    <row r="152" spans="18:20" x14ac:dyDescent="0.3">
       <c r="R152">
         <v>9.0410826452521256E-2</v>
       </c>
@@ -23122,7 +23113,7 @@
         <v>0.32331116236037971</v>
       </c>
     </row>
-    <row r="153" spans="18:20" x14ac:dyDescent="0.25">
+    <row r="153" spans="18:20" x14ac:dyDescent="0.3">
       <c r="R153">
         <v>9.4294612309518466E-2</v>
       </c>
@@ -23133,7 +23124,7 @@
         <v>0.34281098051608705</v>
       </c>
     </row>
-    <row r="154" spans="18:20" x14ac:dyDescent="0.25">
+    <row r="154" spans="18:20" x14ac:dyDescent="0.3">
       <c r="R154">
         <v>9.8178398166515676E-2</v>
       </c>
@@ -23144,7 +23135,7 @@
         <v>0.36218620891543285</v>
       </c>
     </row>
-    <row r="155" spans="18:20" x14ac:dyDescent="0.25">
+    <row r="155" spans="18:20" x14ac:dyDescent="0.3">
       <c r="R155">
         <v>0.1</v>
       </c>
@@ -23155,7 +23146,7 @@
         <v>0.37122754280711856</v>
       </c>
     </row>
-    <row r="156" spans="18:20" x14ac:dyDescent="0.25">
+    <row r="156" spans="18:20" x14ac:dyDescent="0.3">
       <c r="R156">
         <v>0.10182160183348433</v>
       </c>
@@ -23166,7 +23157,7 @@
         <v>0.38023872961192229</v>
       </c>
     </row>
-    <row r="157" spans="18:20" x14ac:dyDescent="0.25">
+    <row r="157" spans="18:20" x14ac:dyDescent="0.3">
       <c r="R157">
         <v>0.10364320366696866</v>
       </c>
@@ -23177,7 +23168,7 @@
         <v>0.38921921204619192</v>
       </c>
     </row>
-    <row r="158" spans="18:20" x14ac:dyDescent="0.25">
+    <row r="158" spans="18:20" x14ac:dyDescent="0.3">
       <c r="R158">
         <v>0.10546480550045299</v>
       </c>
@@ -23188,7 +23179,7 @@
         <v>0.39816877929187022</v>
       </c>
     </row>
-    <row r="159" spans="18:20" x14ac:dyDescent="0.25">
+    <row r="159" spans="18:20" x14ac:dyDescent="0.3">
       <c r="R159">
         <v>0.10728640733393732</v>
       </c>
@@ -23199,7 +23190,7 @@
         <v>0.40708758654669275</v>
       </c>
     </row>
-    <row r="160" spans="18:20" x14ac:dyDescent="0.25">
+    <row r="160" spans="18:20" x14ac:dyDescent="0.3">
       <c r="R160">
         <v>0.11225044586203323</v>
       </c>
@@ -23210,7 +23201,7 @@
         <v>0.43124215656762477</v>
       </c>
     </row>
-    <row r="161" spans="18:20" x14ac:dyDescent="0.25">
+    <row r="161" spans="18:20" x14ac:dyDescent="0.3">
       <c r="R161">
         <v>0.11721448439012913</v>
       </c>
@@ -23221,7 +23212,7 @@
         <v>0.45518663893620825</v>
       </c>
     </row>
-    <row r="162" spans="18:20" x14ac:dyDescent="0.25">
+    <row r="162" spans="18:20" x14ac:dyDescent="0.3">
       <c r="R162">
         <v>0.12</v>
       </c>
@@ -23232,7 +23223,7 @@
         <v>0.46853562853379138</v>
       </c>
     </row>
-    <row r="163" spans="18:20" x14ac:dyDescent="0.25">
+    <row r="163" spans="18:20" x14ac:dyDescent="0.3">
       <c r="R163">
         <v>0.12278551560987086</v>
       </c>
@@ -23243,7 +23234,7 @@
         <v>0.48182739046882705</v>
       </c>
     </row>
-    <row r="164" spans="18:20" x14ac:dyDescent="0.25">
+    <row r="164" spans="18:20" x14ac:dyDescent="0.3">
       <c r="R164">
         <v>0.12557103121974172</v>
       </c>
@@ -23254,7 +23245,7 @@
         <v>0.49506596062279851</v>
       </c>
     </row>
-    <row r="165" spans="18:20" x14ac:dyDescent="0.25">
+    <row r="165" spans="18:20" x14ac:dyDescent="0.3">
       <c r="R165">
         <v>0.12835654682961259</v>
       </c>
@@ -23265,7 +23256,7 @@
         <v>0.50825544936999911</v>
       </c>
     </row>
-    <row r="166" spans="18:20" x14ac:dyDescent="0.25">
+    <row r="166" spans="18:20" x14ac:dyDescent="0.3">
       <c r="R166">
         <v>0.13649998830617247</v>
       </c>
@@ -23276,7 +23267,7 @@
         <v>0.54657041860599875</v>
       </c>
     </row>
-    <row r="167" spans="18:20" x14ac:dyDescent="0.25">
+    <row r="167" spans="18:20" x14ac:dyDescent="0.3">
       <c r="R167">
         <v>0.14000000000000001</v>
       </c>
@@ -23287,7 +23278,7 @@
         <v>0.56294438762356247</v>
       </c>
     </row>
-    <row r="168" spans="18:20" x14ac:dyDescent="0.25">
+    <row r="168" spans="18:20" x14ac:dyDescent="0.3">
       <c r="R168">
         <v>0.14350001169382756</v>
       </c>
@@ -23298,7 +23289,7 @@
         <v>0.57927287420904161</v>
       </c>
     </row>
-    <row r="169" spans="18:20" x14ac:dyDescent="0.25">
+    <row r="169" spans="18:20" x14ac:dyDescent="0.3">
       <c r="R169">
         <v>0.14700002338765511</v>
       </c>
@@ -23309,7 +23300,7 @@
         <v>0.59556240765284763</v>
       </c>
     </row>
-    <row r="170" spans="18:20" x14ac:dyDescent="0.25">
+    <row r="170" spans="18:20" x14ac:dyDescent="0.3">
       <c r="R170">
         <v>0.15050003508148266</v>
       </c>
@@ -23320,7 +23311,7 @@
         <v>0.61181870448733022</v>
       </c>
     </row>
-    <row r="171" spans="18:20" x14ac:dyDescent="0.25">
+    <row r="171" spans="18:20" x14ac:dyDescent="0.3">
       <c r="R171">
         <v>0.15334976740598016</v>
       </c>
@@ -23331,7 +23322,7 @@
         <v>0.62500936669939122</v>
       </c>
     </row>
-    <row r="172" spans="18:20" x14ac:dyDescent="0.25">
+    <row r="172" spans="18:20" x14ac:dyDescent="0.3">
       <c r="R172">
         <v>0.15583807449804907</v>
       </c>
@@ -23342,7 +23333,7 @@
         <v>0.63645506205384184</v>
       </c>
     </row>
-    <row r="173" spans="18:20" x14ac:dyDescent="0.25">
+    <row r="173" spans="18:20" x14ac:dyDescent="0.3">
       <c r="R173">
         <v>0.15761112961337387</v>
       </c>
@@ -23353,7 +23344,7 @@
         <v>0.64456273130304709</v>
       </c>
     </row>
-    <row r="174" spans="18:20" x14ac:dyDescent="0.25">
+    <row r="174" spans="18:20" x14ac:dyDescent="0.3">
       <c r="R174">
         <v>0.15876843503056287</v>
       </c>
@@ -23364,7 +23355,7 @@
         <v>0.64983406420102519</v>
       </c>
     </row>
-    <row r="175" spans="18:20" x14ac:dyDescent="0.25">
+    <row r="175" spans="18:20" x14ac:dyDescent="0.3">
       <c r="R175">
         <v>0.15918824579032559</v>
       </c>
@@ -23375,7 +23366,7 @@
         <v>0.65174261929975597</v>
       </c>
     </row>
-    <row r="176" spans="18:20" x14ac:dyDescent="0.25">
+    <row r="176" spans="18:20" x14ac:dyDescent="0.3">
       <c r="R176">
         <v>0.15960805655008831</v>
       </c>
@@ -23386,7 +23377,7 @@
         <v>0.6536496398613032</v>
       </c>
     </row>
-    <row r="177" spans="18:20" x14ac:dyDescent="0.25">
+    <row r="177" spans="18:20" x14ac:dyDescent="0.3">
       <c r="R177">
         <v>0.16</v>
       </c>
@@ -23397,7 +23388,7 @@
         <v>0.65542874699964226</v>
       </c>
     </row>
-    <row r="178" spans="18:20" x14ac:dyDescent="0.25">
+    <row r="178" spans="18:20" x14ac:dyDescent="0.3">
       <c r="R178">
         <v>0.1603919434499117</v>
       </c>
@@ -23408,7 +23399,7 @@
         <v>0.65720658580530422</v>
       </c>
     </row>
-    <row r="179" spans="18:20" x14ac:dyDescent="0.25">
+    <row r="179" spans="18:20" x14ac:dyDescent="0.3">
       <c r="R179">
         <v>0.1607838868998234</v>
       </c>
@@ -23419,7 +23410,7 @@
         <v>0.65898316087841824</v>
       </c>
     </row>
-    <row r="180" spans="18:20" x14ac:dyDescent="0.25">
+    <row r="180" spans="18:20" x14ac:dyDescent="0.3">
       <c r="R180">
         <v>0.16117583034973509</v>
       </c>
@@ -23430,7 +23421,7 @@
         <v>0.66075848104235391</v>
       </c>
     </row>
-    <row r="181" spans="18:20" x14ac:dyDescent="0.25">
+    <row r="181" spans="18:20" x14ac:dyDescent="0.3">
       <c r="R181">
         <v>0.1629775036449177</v>
       </c>
@@ -23441,7 +23432,7 @@
         <v>0.66890352178322576</v>
       </c>
     </row>
-    <row r="182" spans="18:20" x14ac:dyDescent="0.25">
+    <row r="182" spans="18:20" x14ac:dyDescent="0.3">
       <c r="R182">
         <v>0.1647791769401003</v>
       </c>
@@ -23452,7 +23443,7 @@
         <v>0.67702331430757035</v>
       </c>
     </row>
-    <row r="183" spans="18:20" x14ac:dyDescent="0.25">
+    <row r="183" spans="18:20" x14ac:dyDescent="0.3">
       <c r="R183">
         <v>0.16658085023528291</v>
       </c>
@@ -23463,7 +23454,7 @@
         <v>0.68512135552445397</v>
       </c>
     </row>
-    <row r="184" spans="18:20" x14ac:dyDescent="0.25">
+    <row r="184" spans="18:20" x14ac:dyDescent="0.3">
       <c r="R184">
         <v>0.16838252353046551</v>
       </c>
@@ -23474,7 +23465,7 @@
         <v>0.69320068953039815</v>
       </c>
     </row>
-    <row r="185" spans="18:20" x14ac:dyDescent="0.25">
+    <row r="185" spans="18:20" x14ac:dyDescent="0.3">
       <c r="R185">
         <v>0.17028822108396738</v>
       </c>
@@ -23485,7 +23476,7 @@
         <v>0.70172754741981347</v>
       </c>
     </row>
-    <row r="186" spans="18:20" x14ac:dyDescent="0.25">
+    <row r="186" spans="18:20" x14ac:dyDescent="0.3">
       <c r="R186">
         <v>0.17219391863746925</v>
       </c>
@@ -23496,7 +23487,7 @@
         <v>0.71023917360030087</v>
       </c>
     </row>
-    <row r="187" spans="18:20" x14ac:dyDescent="0.25">
+    <row r="187" spans="18:20" x14ac:dyDescent="0.3">
       <c r="R187">
         <v>0.17409961619097111</v>
       </c>
@@ -23507,7 +23498,7 @@
         <v>0.71874106677911076</v>
       </c>
     </row>
-    <row r="188" spans="18:20" x14ac:dyDescent="0.25">
+    <row r="188" spans="18:20" x14ac:dyDescent="0.3">
       <c r="R188">
         <v>0.17600531374447298</v>
       </c>
@@ -23518,7 +23509,7 @@
         <v>0.72723515128451854</v>
       </c>
     </row>
-    <row r="189" spans="18:20" x14ac:dyDescent="0.25">
+    <row r="189" spans="18:20" x14ac:dyDescent="0.3">
       <c r="R189">
         <v>0.1785024876704053</v>
       </c>
@@ -23529,7 +23520,7 @@
         <v>0.73835299734952731</v>
       </c>
     </row>
-    <row r="190" spans="18:20" x14ac:dyDescent="0.25">
+    <row r="190" spans="18:20" x14ac:dyDescent="0.3">
       <c r="R190">
         <v>0.18</v>
       </c>
@@ -23540,7 +23531,7 @@
         <v>0.74501192891772483</v>
       </c>
     </row>
-    <row r="191" spans="18:20" x14ac:dyDescent="0.25">
+    <row r="191" spans="18:20" x14ac:dyDescent="0.3">
       <c r="R191">
         <v>0.1805431557342127</v>
       </c>
@@ -23551,7 +23542,7 @@
         <v>0.74742522019950641</v>
       </c>
     </row>
-    <row r="192" spans="18:20" x14ac:dyDescent="0.25">
+    <row r="192" spans="18:20" x14ac:dyDescent="0.3">
       <c r="R192">
         <v>0.18108631146842541</v>
       </c>
@@ -23562,7 +23553,7 @@
         <v>0.74983744628516114</v>
       </c>
     </row>
-    <row r="193" spans="18:20" x14ac:dyDescent="0.25">
+    <row r="193" spans="18:20" x14ac:dyDescent="0.3">
       <c r="R193">
         <v>0.18162946720263812</v>
       </c>
@@ -23573,7 +23564,7 @@
         <v>0.75224863701509648</v>
       </c>
     </row>
-    <row r="194" spans="18:20" x14ac:dyDescent="0.25">
+    <row r="194" spans="18:20" x14ac:dyDescent="0.3">
       <c r="R194">
         <v>0.18217262293685083</v>
       </c>
@@ -23584,7 +23575,7 @@
         <v>0.75465880584295153</v>
       </c>
     </row>
-    <row r="195" spans="18:20" x14ac:dyDescent="0.25">
+    <row r="195" spans="18:20" x14ac:dyDescent="0.3">
       <c r="R195">
         <v>0.18271577867106353</v>
       </c>
@@ -23595,7 +23586,7 @@
         <v>0.75706795471973543</v>
       </c>
     </row>
-    <row r="196" spans="18:20" x14ac:dyDescent="0.25">
+    <row r="196" spans="18:20" x14ac:dyDescent="0.3">
       <c r="R196">
         <v>0.18557875682798169</v>
       </c>
@@ -23606,7 +23597,7 @@
         <v>0.76974980275935589</v>
       </c>
     </row>
-    <row r="197" spans="18:20" x14ac:dyDescent="0.25">
+    <row r="197" spans="18:20" x14ac:dyDescent="0.3">
       <c r="R197">
         <v>0.18844173498489986</v>
       </c>
@@ -23617,7 +23608,7 @@
         <v>0.7824014057317159</v>
       </c>
     </row>
-    <row r="198" spans="18:20" x14ac:dyDescent="0.25">
+    <row r="198" spans="18:20" x14ac:dyDescent="0.3">
       <c r="R198">
         <v>0.19130471314181802</v>
       </c>
@@ -23628,7 +23619,7 @@
         <v>0.79502215896362394</v>
       </c>
     </row>
-    <row r="199" spans="18:20" x14ac:dyDescent="0.25">
+    <row r="199" spans="18:20" x14ac:dyDescent="0.3">
       <c r="R199">
         <v>0.19416769129873618</v>
       </c>
@@ -23639,7 +23630,7 @@
         <v>0.80761302720263295</v>
       </c>
     </row>
-    <row r="200" spans="18:20" x14ac:dyDescent="0.25">
+    <row r="200" spans="18:20" x14ac:dyDescent="0.3">
       <c r="R200">
         <v>0.1951972621106752</v>
       </c>
@@ -23650,7 +23641,7 @@
         <v>0.81213293462696612</v>
       </c>
     </row>
-    <row r="201" spans="18:20" x14ac:dyDescent="0.25">
+    <row r="201" spans="18:20" x14ac:dyDescent="0.3">
       <c r="R201">
         <v>0.19598146239398898</v>
       </c>
@@ -23661,7 +23652,7 @@
         <v>0.81556891314271773</v>
       </c>
     </row>
-    <row r="202" spans="18:20" x14ac:dyDescent="0.25">
+    <row r="202" spans="18:20" x14ac:dyDescent="0.3">
       <c r="R202">
         <v>0.19676566267730275</v>
       </c>
@@ -23672,7 +23663,7 @@
         <v>0.81899786566216548</v>
       </c>
     </row>
-    <row r="203" spans="18:20" x14ac:dyDescent="0.25">
+    <row r="203" spans="18:20" x14ac:dyDescent="0.3">
       <c r="R203">
         <v>0.19754986296061652</v>
       </c>
@@ -23683,7 +23674,7 @@
         <v>0.82241988964753521</v>
       </c>
     </row>
-    <row r="204" spans="18:20" x14ac:dyDescent="0.25">
+    <row r="204" spans="18:20" x14ac:dyDescent="0.3">
       <c r="R204">
         <v>0.19924536427081849</v>
       </c>
@@ -23694,7 +23685,7 @@
         <v>0.82979061570409129</v>
       </c>
     </row>
-    <row r="205" spans="18:20" x14ac:dyDescent="0.25">
+    <row r="205" spans="18:20" x14ac:dyDescent="0.3">
       <c r="R205">
         <v>0.2</v>
       </c>
@@ -23705,7 +23696,7 @@
         <v>0.8330643438137999</v>
       </c>
     </row>
-    <row r="206" spans="18:20" x14ac:dyDescent="0.25">
+    <row r="206" spans="18:20" x14ac:dyDescent="0.3">
       <c r="R206">
         <v>0.20075463572918154</v>
       </c>
@@ -23716,7 +23707,7 @@
         <v>0.83633224191560807</v>
       </c>
     </row>
-    <row r="207" spans="18:20" x14ac:dyDescent="0.25">
+    <row r="207" spans="18:20" x14ac:dyDescent="0.3">
       <c r="R207">
         <v>0.20150927145836306</v>
       </c>
@@ -23727,7 +23718,7 @@
         <v>0.83959461499671217</v>
       </c>
     </row>
-    <row r="208" spans="18:20" x14ac:dyDescent="0.25">
+    <row r="208" spans="18:20" x14ac:dyDescent="0.3">
       <c r="R208">
         <v>0.20235827279714005</v>
       </c>
@@ -23738,7 +23729,7 @@
         <v>0.8432598078108331</v>
       </c>
     </row>
-    <row r="209" spans="18:20" x14ac:dyDescent="0.25">
+    <row r="209" spans="18:20" x14ac:dyDescent="0.3">
       <c r="R209">
         <v>0.20320727413591705</v>
       </c>
@@ -23749,7 +23740,7 @@
         <v>0.84691931660072051</v>
       </c>
     </row>
-    <row r="210" spans="18:20" x14ac:dyDescent="0.25">
+    <row r="210" spans="18:20" x14ac:dyDescent="0.3">
       <c r="R210">
         <v>0.20405627547469404</v>
       </c>
@@ -23760,7 +23751,7 @@
         <v>0.85057333756253772</v>
       </c>
     </row>
-    <row r="211" spans="18:20" x14ac:dyDescent="0.25">
+    <row r="211" spans="18:20" x14ac:dyDescent="0.3">
       <c r="R211">
         <v>0.20490527681347104</v>
       </c>
@@ -23771,7 +23762,7 @@
         <v>0.85422223194020308</v>
       </c>
     </row>
-    <row r="212" spans="18:20" x14ac:dyDescent="0.25">
+    <row r="212" spans="18:20" x14ac:dyDescent="0.3">
       <c r="R212">
         <v>0.205860020468176</v>
       </c>
@@ -23782,7 +23773,7 @@
         <v>0.85831811024320537</v>
       </c>
     </row>
-    <row r="213" spans="18:20" x14ac:dyDescent="0.25">
+    <row r="213" spans="18:20" x14ac:dyDescent="0.3">
       <c r="R213">
         <v>0.20681476412288097</v>
       </c>
@@ -23793,7 +23784,7 @@
         <v>0.86240780198616829</v>
       </c>
     </row>
-    <row r="214" spans="18:20" x14ac:dyDescent="0.25">
+    <row r="214" spans="18:20" x14ac:dyDescent="0.3">
       <c r="R214">
         <v>0.20776950777758593</v>
       </c>
@@ -23804,7 +23795,7 @@
         <v>0.86649158853013741</v>
       </c>
     </row>
-    <row r="215" spans="18:20" x14ac:dyDescent="0.25">
+    <row r="215" spans="18:20" x14ac:dyDescent="0.3">
       <c r="R215">
         <v>0.2097117161196268</v>
       </c>
@@ -23815,7 +23806,7 @@
         <v>0.87478360159956381</v>
       </c>
     </row>
-    <row r="216" spans="18:20" x14ac:dyDescent="0.25">
+    <row r="216" spans="18:20" x14ac:dyDescent="0.3">
       <c r="R216">
         <v>0.21165392446166767</v>
       </c>
@@ -23826,7 +23817,7 @@
         <v>0.8830536075471116</v>
       </c>
     </row>
-    <row r="217" spans="18:20" x14ac:dyDescent="0.25">
+    <row r="217" spans="18:20" x14ac:dyDescent="0.3">
       <c r="R217">
         <v>0.21318276170100725</v>
       </c>
@@ -23837,7 +23828,7 @@
         <v>0.88954995481480914</v>
       </c>
     </row>
-    <row r="218" spans="18:20" x14ac:dyDescent="0.25">
+    <row r="218" spans="18:20" x14ac:dyDescent="0.3">
       <c r="R218">
         <v>0.21471159894034683</v>
       </c>
@@ -23848,7 +23839,7 @@
         <v>0.89603640698131848</v>
       </c>
     </row>
-    <row r="219" spans="18:20" x14ac:dyDescent="0.25">
+    <row r="219" spans="18:20" x14ac:dyDescent="0.3">
       <c r="R219">
         <v>0.21624043617968641</v>
       </c>
@@ -23859,7 +23850,7 @@
         <v>0.9025132246791765</v>
       </c>
     </row>
-    <row r="220" spans="18:20" x14ac:dyDescent="0.25">
+    <row r="220" spans="18:20" x14ac:dyDescent="0.3">
       <c r="R220">
         <v>0.21776927341902599</v>
       </c>
@@ -23870,7 +23861,7 @@
         <v>0.90898015965865842</v>
       </c>
     </row>
-    <row r="221" spans="18:20" x14ac:dyDescent="0.25">
+    <row r="221" spans="18:20" x14ac:dyDescent="0.3">
       <c r="R221">
         <v>0.22</v>
       </c>
@@ -23881,7 +23872,7 @@
         <v>0.91839772846161249</v>
       </c>
     </row>
-    <row r="222" spans="18:20" x14ac:dyDescent="0.25">
+    <row r="222" spans="18:20" x14ac:dyDescent="0.3">
       <c r="R222">
         <v>0.22223072658097401</v>
       </c>
@@ -23892,7 +23883,7 @@
         <v>0.92779307163740299</v>
       </c>
     </row>
-    <row r="223" spans="18:20" x14ac:dyDescent="0.25">
+    <row r="223" spans="18:20" x14ac:dyDescent="0.3">
       <c r="R223">
         <v>0.22446145316194802</v>
       </c>
@@ -23903,7 +23894,7 @@
         <v>0.93716575277239578</v>
       </c>
     </row>
-    <row r="224" spans="18:20" x14ac:dyDescent="0.25">
+    <row r="224" spans="18:20" x14ac:dyDescent="0.3">
       <c r="R224">
         <v>0.22669217974292202</v>
       </c>
@@ -23914,7 +23905,7 @@
         <v>0.94651550731630252</v>
       </c>
     </row>
-    <row r="225" spans="18:20" x14ac:dyDescent="0.25">
+    <row r="225" spans="18:20" x14ac:dyDescent="0.3">
       <c r="R225">
         <v>0.23376721530409275</v>
       </c>
@@ -23925,7 +23916,7 @@
         <v>0.97601820400495232</v>
       </c>
     </row>
-    <row r="226" spans="18:20" x14ac:dyDescent="0.25">
+    <row r="226" spans="18:20" x14ac:dyDescent="0.3">
       <c r="R226">
         <v>0.24</v>
       </c>
@@ -23936,7 +23927,7 @@
         <v>1.0018200910930481</v>
       </c>
     </row>
-    <row r="227" spans="18:20" x14ac:dyDescent="0.25">
+    <row r="227" spans="18:20" x14ac:dyDescent="0.3">
       <c r="R227">
         <v>0.24186983540877216</v>
       </c>
@@ -23947,7 +23938,7 @@
         <v>1.0095267096125813</v>
       </c>
     </row>
-    <row r="228" spans="18:20" x14ac:dyDescent="0.25">
+    <row r="228" spans="18:20" x14ac:dyDescent="0.3">
       <c r="R228">
         <v>0.24373967081754433</v>
       </c>
@@ -23958,7 +23949,7 @@
         <v>1.0172181674661882</v>
       </c>
     </row>
-    <row r="229" spans="18:20" x14ac:dyDescent="0.25">
+    <row r="229" spans="18:20" x14ac:dyDescent="0.3">
       <c r="R229">
         <v>0.2456095062263165</v>
       </c>
@@ -23969,7 +23960,7 @@
         <v>1.0248948779029865</v>
       </c>
     </row>
-    <row r="230" spans="18:20" x14ac:dyDescent="0.25">
+    <row r="230" spans="18:20" x14ac:dyDescent="0.3">
       <c r="R230">
         <v>0.24747934163508867</v>
       </c>
@@ -23980,7 +23971,7 @@
         <v>1.0325572304517578</v>
       </c>
     </row>
-    <row r="231" spans="18:20" x14ac:dyDescent="0.25">
+    <row r="231" spans="18:20" x14ac:dyDescent="0.3">
       <c r="R231">
         <v>0.24934917704386084</v>
       </c>
@@ -23991,7 +23982,7 @@
         <v>1.0402056384477216</v>
       </c>
     </row>
-    <row r="232" spans="18:20" x14ac:dyDescent="0.25">
+    <row r="232" spans="18:20" x14ac:dyDescent="0.3">
       <c r="R232">
         <v>0.2582608934255784</v>
       </c>
@@ -24002,7 +23993,7 @@
         <v>1.0764846363799121</v>
       </c>
     </row>
-    <row r="233" spans="18:20" x14ac:dyDescent="0.25">
+    <row r="233" spans="18:20" x14ac:dyDescent="0.3">
       <c r="R233">
         <v>0.26</v>
       </c>
@@ -24013,7 +24004,7 @@
         <v>1.0835307305440876</v>
       </c>
     </row>
-    <row r="234" spans="18:20" x14ac:dyDescent="0.25">
+    <row r="234" spans="18:20" x14ac:dyDescent="0.3">
       <c r="R234">
         <v>0.26173910657442162</v>
       </c>
@@ -24024,7 +24015,7 @@
         <v>1.0905669707021639</v>
       </c>
     </row>
-    <row r="235" spans="18:20" x14ac:dyDescent="0.25">
+    <row r="235" spans="18:20" x14ac:dyDescent="0.3">
       <c r="R235">
         <v>0.26347821314884323</v>
       </c>
@@ -24035,7 +24026,7 @@
         <v>1.0975935701319584</v>
       </c>
     </row>
-    <row r="236" spans="18:20" x14ac:dyDescent="0.25">
+    <row r="236" spans="18:20" x14ac:dyDescent="0.3">
       <c r="R236">
         <v>0.26521731972326484</v>
       </c>
@@ -24046,7 +24037,7 @@
         <v>1.1046107301377868</v>
       </c>
     </row>
-    <row r="237" spans="18:20" x14ac:dyDescent="0.25">
+    <row r="237" spans="18:20" x14ac:dyDescent="0.3">
       <c r="R237">
         <v>0.26965212380628539</v>
       </c>
@@ -24057,7 +24048,7 @@
         <v>1.122463820666983</v>
       </c>
     </row>
-    <row r="238" spans="18:20" x14ac:dyDescent="0.25">
+    <row r="238" spans="18:20" x14ac:dyDescent="0.3">
       <c r="R238">
         <v>0.27408692788930594</v>
       </c>
@@ -24068,7 +24059,7 @@
         <v>1.140260969603561</v>
       </c>
     </row>
-    <row r="239" spans="18:20" x14ac:dyDescent="0.25">
+    <row r="239" spans="18:20" x14ac:dyDescent="0.3">
       <c r="R239">
         <v>0.27852173197232649</v>
       </c>
@@ -24079,7 +24070,7 @@
         <v>1.1580077440424255</v>
       </c>
     </row>
-    <row r="240" spans="18:20" x14ac:dyDescent="0.25">
+    <row r="240" spans="18:20" x14ac:dyDescent="0.3">
       <c r="R240">
         <v>0.28000000000000003</v>
       </c>
@@ -24090,7 +24081,7 @@
         <v>1.1639123189562328</v>
       </c>
     </row>
-    <row r="241" spans="18:20" x14ac:dyDescent="0.25">
+    <row r="241" spans="18:20" x14ac:dyDescent="0.3">
       <c r="R241">
         <v>0.28147826802767356</v>
       </c>
@@ -24101,7 +24092,7 @@
         <v>1.1698114346973547</v>
       </c>
     </row>
-    <row r="242" spans="18:20" x14ac:dyDescent="0.25">
+    <row r="242" spans="18:20" x14ac:dyDescent="0.3">
       <c r="R242">
         <v>0.2829565360553471</v>
       </c>
@@ -24112,7 +24103,7 @@
         <v>1.1757050235122883</v>
       </c>
     </row>
-    <row r="243" spans="18:20" x14ac:dyDescent="0.25">
+    <row r="243" spans="18:20" x14ac:dyDescent="0.3">
       <c r="R243">
         <v>0.28443480408302063</v>
       </c>
@@ -24123,7 +24114,7 @@
         <v>1.1815930135739285</v>
       </c>
     </row>
-    <row r="244" spans="18:20" x14ac:dyDescent="0.25">
+    <row r="244" spans="18:20" x14ac:dyDescent="0.3">
       <c r="R244">
         <v>0.29466316508490481</v>
       </c>
@@ -24134,7 +24125,7 @@
         <v>1.2221728525139128</v>
       </c>
     </row>
-    <row r="245" spans="18:20" x14ac:dyDescent="0.25">
+    <row r="245" spans="18:20" x14ac:dyDescent="0.3">
       <c r="R245">
         <v>0.3</v>
       </c>
@@ -24145,7 +24136,7 @@
         <v>1.2432338991778811</v>
       </c>
     </row>
-    <row r="246" spans="18:20" x14ac:dyDescent="0.25">
+    <row r="246" spans="18:20" x14ac:dyDescent="0.3">
       <c r="R246">
         <v>0.30533683491509517</v>
       </c>
@@ -24156,7 +24147,7 @@
         <v>1.2642144536473054</v>
       </c>
     </row>
-    <row r="247" spans="18:20" x14ac:dyDescent="0.25">
+    <row r="247" spans="18:20" x14ac:dyDescent="0.3">
       <c r="R247">
         <v>0.31067366983019035</v>
       </c>
@@ -24167,7 +24158,7 @@
         <v>1.2851122984342029</v>
       </c>
     </row>
-    <row r="248" spans="18:20" x14ac:dyDescent="0.25">
+    <row r="248" spans="18:20" x14ac:dyDescent="0.3">
       <c r="R248">
         <v>0.31601050474528553</v>
       </c>
@@ -24178,7 +24169,7 @@
         <v>1.3059253524994556</v>
       </c>
     </row>
-    <row r="249" spans="18:20" x14ac:dyDescent="0.25">
+    <row r="249" spans="18:20" x14ac:dyDescent="0.3">
       <c r="R249">
         <v>0.32</v>
       </c>
@@ -24189,7 +24180,7 @@
         <v>1.3214274598580031</v>
       </c>
     </row>
-    <row r="250" spans="18:20" x14ac:dyDescent="0.25">
+    <row r="250" spans="18:20" x14ac:dyDescent="0.3">
       <c r="R250">
         <v>0.32119684857641434</v>
       </c>
@@ -24200,7 +24191,7 @@
         <v>1.3260685406345041</v>
       </c>
     </row>
-    <row r="251" spans="18:20" x14ac:dyDescent="0.25">
+    <row r="251" spans="18:20" x14ac:dyDescent="0.3">
       <c r="R251">
         <v>0.32239369715282867</v>
       </c>
@@ -24211,7 +24202,7 @@
         <v>1.3307051626916739</v>
       </c>
     </row>
-    <row r="252" spans="18:20" x14ac:dyDescent="0.25">
+    <row r="252" spans="18:20" x14ac:dyDescent="0.3">
       <c r="R252">
         <v>0.32359054572924301</v>
       </c>
@@ -24222,7 +24213,7 @@
         <v>1.3353408661666548</v>
       </c>
     </row>
-    <row r="253" spans="18:20" x14ac:dyDescent="0.25">
+    <row r="253" spans="18:20" x14ac:dyDescent="0.3">
       <c r="R253">
         <v>0.32478739430565734</v>
       </c>
@@ -24233,7 +24224,7 @@
         <v>1.3399851637250535</v>
       </c>
     </row>
-    <row r="254" spans="18:20" x14ac:dyDescent="0.25">
+    <row r="254" spans="18:20" x14ac:dyDescent="0.3">
       <c r="R254">
         <v>0.3257551175318279</v>
       </c>
@@ -24244,7 +24235,7 @@
         <v>1.3437513844057252</v>
       </c>
     </row>
-    <row r="255" spans="18:20" x14ac:dyDescent="0.25">
+    <row r="255" spans="18:20" x14ac:dyDescent="0.3">
       <c r="R255">
         <v>0.32672284075799846</v>
       </c>
@@ -24255,7 +24246,7 @@
         <v>1.3475276058462655</v>
       </c>
     </row>
-    <row r="256" spans="18:20" x14ac:dyDescent="0.25">
+    <row r="256" spans="18:20" x14ac:dyDescent="0.3">
       <c r="R256">
         <v>0.32769056398416901</v>
       </c>
@@ -24266,7 +24257,7 @@
         <v>1.3513126509643736</v>
       </c>
     </row>
-    <row r="257" spans="18:20" x14ac:dyDescent="0.25">
+    <row r="257" spans="18:20" x14ac:dyDescent="0.3">
       <c r="R257">
         <v>0.32865828721033957</v>
       </c>
@@ -24277,7 +24268,7 @@
         <v>1.3551056724636688</v>
       </c>
     </row>
-    <row r="258" spans="18:20" x14ac:dyDescent="0.25">
+    <row r="258" spans="18:20" x14ac:dyDescent="0.3">
       <c r="R258">
         <v>0.32962601043651013</v>
       </c>
@@ -24288,7 +24279,7 @@
         <v>1.3589062454482819</v>
       </c>
     </row>
-    <row r="259" spans="18:20" x14ac:dyDescent="0.25">
+    <row r="259" spans="18:20" x14ac:dyDescent="0.3">
       <c r="R259">
         <v>0.3320942412955406</v>
       </c>
@@ -24299,7 +24290,7 @@
         <v>1.3686310679584945</v>
       </c>
     </row>
-    <row r="260" spans="18:20" x14ac:dyDescent="0.25">
+    <row r="260" spans="18:20" x14ac:dyDescent="0.3">
       <c r="R260">
         <v>0.33456247215457108</v>
       </c>
@@ -24310,7 +24301,7 @@
         <v>1.378397261476203</v>
       </c>
     </row>
-    <row r="261" spans="18:20" x14ac:dyDescent="0.25">
+    <row r="261" spans="18:20" x14ac:dyDescent="0.3">
       <c r="R261">
         <v>0.33703070301360155</v>
       </c>
@@ -24321,7 +24312,7 @@
         <v>1.3881970776230674</v>
       </c>
     </row>
-    <row r="262" spans="18:20" x14ac:dyDescent="0.25">
+    <row r="262" spans="18:20" x14ac:dyDescent="0.3">
       <c r="R262">
         <v>0.33949893387263202</v>
       </c>
@@ -24332,7 +24323,7 @@
         <v>1.3980200346622178</v>
       </c>
     </row>
-    <row r="263" spans="18:20" x14ac:dyDescent="0.25">
+    <row r="263" spans="18:20" x14ac:dyDescent="0.3">
       <c r="R263">
         <v>0.34</v>
       </c>
@@ -24343,7 +24334,7 @@
         <v>1.4000162972143064</v>
       </c>
     </row>
-    <row r="264" spans="18:20" x14ac:dyDescent="0.25">
+    <row r="264" spans="18:20" x14ac:dyDescent="0.3">
       <c r="R264">
         <v>0.34050106612736802</v>
       </c>
@@ -24354,7 +24345,7 @@
         <v>1.4020133424871211</v>
       </c>
     </row>
-    <row r="265" spans="18:20" x14ac:dyDescent="0.25">
+    <row r="265" spans="18:20" x14ac:dyDescent="0.3">
       <c r="R265">
         <v>0.34100213225473602</v>
       </c>
@@ -24365,7 +24356,7 @@
         <v>1.4040110898083404</v>
       </c>
     </row>
-    <row r="266" spans="18:20" x14ac:dyDescent="0.25">
+    <row r="266" spans="18:20" x14ac:dyDescent="0.3">
       <c r="R266">
         <v>0.34150319838210402</v>
       </c>
@@ -24376,7 +24367,7 @@
         <v>1.4060094774136287</v>
       </c>
     </row>
-    <row r="267" spans="18:20" x14ac:dyDescent="0.25">
+    <row r="267" spans="18:20" x14ac:dyDescent="0.3">
       <c r="R267">
         <v>0.34200426450947202</v>
       </c>
@@ -24387,7 +24378,7 @@
         <v>1.4080084821650543</v>
       </c>
     </row>
-    <row r="268" spans="18:20" x14ac:dyDescent="0.25">
+    <row r="268" spans="18:20" x14ac:dyDescent="0.3">
       <c r="R268">
         <v>0.34438019726359209</v>
       </c>
@@ -24398,7 +24389,7 @@
         <v>1.4174952866089989</v>
       </c>
     </row>
-    <row r="269" spans="18:20" x14ac:dyDescent="0.25">
+    <row r="269" spans="18:20" x14ac:dyDescent="0.3">
       <c r="R269">
         <v>0.34675613001771216</v>
       </c>
@@ -24409,7 +24400,7 @@
         <v>1.4269946164051746</v>
       </c>
     </row>
-    <row r="270" spans="18:20" x14ac:dyDescent="0.25">
+    <row r="270" spans="18:20" x14ac:dyDescent="0.3">
       <c r="R270">
         <v>0.34913206277183223</v>
       </c>
@@ -24420,7 +24411,7 @@
         <v>1.4365051951108403</v>
       </c>
     </row>
-    <row r="271" spans="18:20" x14ac:dyDescent="0.25">
+    <row r="271" spans="18:20" x14ac:dyDescent="0.3">
       <c r="R271">
         <v>0.34984484259806825</v>
       </c>
@@ -24431,7 +24422,7 @@
         <v>1.439358587384211</v>
       </c>
     </row>
-    <row r="272" spans="18:20" x14ac:dyDescent="0.25">
+    <row r="272" spans="18:20" x14ac:dyDescent="0.3">
       <c r="R272">
         <v>0.35055762242430427</v>
       </c>
@@ -24442,7 +24433,7 @@
         <v>1.4422077232816646</v>
       </c>
     </row>
-    <row r="273" spans="18:20" x14ac:dyDescent="0.25">
+    <row r="273" spans="18:20" x14ac:dyDescent="0.3">
       <c r="R273">
         <v>0.35127040225054029</v>
       </c>
@@ -24453,7 +24444,7 @@
         <v>1.4450511522930212</v>
       </c>
     </row>
-    <row r="274" spans="18:20" x14ac:dyDescent="0.25">
+    <row r="274" spans="18:20" x14ac:dyDescent="0.3">
       <c r="R274">
         <v>0.35198318207677631</v>
       </c>
@@ -24464,7 +24455,7 @@
         <v>1.4478885599956981</v>
       </c>
     </row>
-    <row r="275" spans="18:20" x14ac:dyDescent="0.25">
+    <row r="275" spans="18:20" x14ac:dyDescent="0.3">
       <c r="R275">
         <v>0.3534139086611689</v>
       </c>
@@ -24475,7 +24466,7 @@
         <v>1.4535599934532324</v>
       </c>
     </row>
-    <row r="276" spans="18:20" x14ac:dyDescent="0.25">
+    <row r="276" spans="18:20" x14ac:dyDescent="0.3">
       <c r="R276">
         <v>0.35484463524556148</v>
       </c>
@@ -24486,7 +24477,7 @@
         <v>1.4592100780445767</v>
       </c>
     </row>
-    <row r="277" spans="18:20" x14ac:dyDescent="0.25">
+    <row r="277" spans="18:20" x14ac:dyDescent="0.3">
       <c r="R277">
         <v>0.35627536182995406</v>
       </c>
@@ -24497,7 +24488,7 @@
         <v>1.4648403562523202</v>
       </c>
     </row>
-    <row r="278" spans="18:20" x14ac:dyDescent="0.25">
+    <row r="278" spans="18:20" x14ac:dyDescent="0.3">
       <c r="R278">
         <v>0.35928924097054066</v>
       </c>
@@ -24508,7 +24499,7 @@
         <v>1.4766486181267631</v>
       </c>
     </row>
-    <row r="279" spans="18:20" x14ac:dyDescent="0.25">
+    <row r="279" spans="18:20" x14ac:dyDescent="0.3">
       <c r="R279">
         <v>0.36</v>
       </c>
@@ -24519,7 +24510,7 @@
         <v>1.4794227115477021</v>
       </c>
     </row>
-    <row r="280" spans="18:20" x14ac:dyDescent="0.25">
+    <row r="280" spans="18:20" x14ac:dyDescent="0.3">
       <c r="R280">
         <v>0.36071075902945932</v>
       </c>
@@ -24530,7 +24521,7 @@
         <v>1.4821928781971763</v>
       </c>
     </row>
-    <row r="281" spans="18:20" x14ac:dyDescent="0.25">
+    <row r="281" spans="18:20" x14ac:dyDescent="0.3">
       <c r="R281">
         <v>0.36142151805891864</v>
       </c>
@@ -24541,7 +24532,7 @@
         <v>1.4849591143991052</v>
       </c>
     </row>
-    <row r="282" spans="18:20" x14ac:dyDescent="0.25">
+    <row r="282" spans="18:20" x14ac:dyDescent="0.3">
       <c r="R282">
         <v>0.36213227708837797</v>
       </c>
@@ -24552,7 +24543,7 @@
         <v>1.4877214878049543</v>
       </c>
     </row>
-    <row r="283" spans="18:20" x14ac:dyDescent="0.25">
+    <row r="283" spans="18:20" x14ac:dyDescent="0.3">
       <c r="R283">
         <v>0.36358534862158304</v>
       </c>
@@ -24563,7 +24554,7 @@
         <v>1.4933573387384342</v>
       </c>
     </row>
-    <row r="284" spans="18:20" x14ac:dyDescent="0.25">
+    <row r="284" spans="18:20" x14ac:dyDescent="0.3">
       <c r="R284">
         <v>0.3650384201547881</v>
       </c>
@@ -24574,7 +24565,7 @@
         <v>1.4989800208471871</v>
       </c>
     </row>
-    <row r="285" spans="18:20" x14ac:dyDescent="0.25">
+    <row r="285" spans="18:20" x14ac:dyDescent="0.3">
       <c r="R285">
         <v>0.36649149168799317</v>
       </c>
@@ -24585,7 +24576,7 @@
         <v>1.5045913967724243</v>
       </c>
     </row>
-    <row r="286" spans="18:20" x14ac:dyDescent="0.25">
+    <row r="286" spans="18:20" x14ac:dyDescent="0.3">
       <c r="R286">
         <v>0.36794456322119823</v>
       </c>
@@ -24596,7 +24587,7 @@
         <v>1.5101921655062749</v>
       </c>
     </row>
-    <row r="287" spans="18:20" x14ac:dyDescent="0.25">
+    <row r="287" spans="18:20" x14ac:dyDescent="0.3">
       <c r="R287">
         <v>0.36986087754507252</v>
       </c>
@@ -24607,7 +24598,7 @@
         <v>1.5175624727727919</v>
       </c>
     </row>
-    <row r="288" spans="18:20" x14ac:dyDescent="0.25">
+    <row r="288" spans="18:20" x14ac:dyDescent="0.3">
       <c r="R288">
         <v>0.37177719186894681</v>
       </c>
@@ -24618,7 +24609,7 @@
         <v>1.5249145401288593</v>
       </c>
     </row>
-    <row r="289" spans="18:20" x14ac:dyDescent="0.25">
+    <row r="289" spans="18:20" x14ac:dyDescent="0.3">
       <c r="R289">
         <v>0.3736935061928211</v>
       </c>
@@ -24629,7 +24620,7 @@
         <v>1.5322483054914877</v>
       </c>
     </row>
-    <row r="290" spans="18:20" x14ac:dyDescent="0.25">
+    <row r="290" spans="18:20" x14ac:dyDescent="0.3">
       <c r="R290">
         <v>0.37560982051669539</v>
       </c>
@@ -24640,7 +24631,7 @@
         <v>1.5395636952170948</v>
       </c>
     </row>
-    <row r="291" spans="18:20" x14ac:dyDescent="0.25">
+    <row r="291" spans="18:20" x14ac:dyDescent="0.3">
       <c r="R291">
         <v>0.37875195808799622</v>
       </c>
@@ -24651,7 +24642,7 @@
         <v>1.5514899236502608</v>
       </c>
     </row>
-    <row r="292" spans="18:20" x14ac:dyDescent="0.25">
+    <row r="292" spans="18:20" x14ac:dyDescent="0.3">
       <c r="R292">
         <v>0.38</v>
       </c>
@@ -24662,7 +24653,7 @@
         <v>1.5561973310557855</v>
       </c>
     </row>
-    <row r="293" spans="18:20" x14ac:dyDescent="0.25">
+    <row r="293" spans="18:20" x14ac:dyDescent="0.3">
       <c r="R293">
         <v>0.38124804191200379</v>
       </c>
@@ -24673,7 +24664,7 @@
         <v>1.5608862323072534</v>
       </c>
     </row>
-    <row r="294" spans="18:20" x14ac:dyDescent="0.25">
+    <row r="294" spans="18:20" x14ac:dyDescent="0.3">
       <c r="R294">
         <v>0.38249608382400757</v>
       </c>
@@ -24684,7 +24675,7 @@
         <v>1.5655577619619221</v>
       </c>
     </row>
-    <row r="295" spans="18:20" x14ac:dyDescent="0.25">
+    <row r="295" spans="18:20" x14ac:dyDescent="0.3">
       <c r="R295">
         <v>0.38374412573601135</v>
       </c>
@@ -24695,7 +24686,7 @@
         <v>1.5702125673910872</v>
       </c>
     </row>
-    <row r="296" spans="18:20" x14ac:dyDescent="0.25">
+    <row r="296" spans="18:20" x14ac:dyDescent="0.3">
       <c r="R296">
         <v>0.38499216764801514</v>
       </c>
@@ -24706,7 +24697,7 @@
         <v>1.574850873102108</v>
       </c>
     </row>
-    <row r="297" spans="18:20" x14ac:dyDescent="0.25">
+    <row r="297" spans="18:20" x14ac:dyDescent="0.3">
       <c r="R297">
         <v>0.38903499150522886</v>
       </c>
@@ -24717,7 +24708,7 @@
         <v>1.5897658448914407</v>
       </c>
     </row>
-    <row r="298" spans="18:20" x14ac:dyDescent="0.25">
+    <row r="298" spans="18:20" x14ac:dyDescent="0.3">
       <c r="R298">
         <v>0.39024783866239299</v>
       </c>
@@ -24728,7 +24719,7 @@
         <v>1.5942076839109967</v>
       </c>
     </row>
-    <row r="299" spans="18:20" x14ac:dyDescent="0.25">
+    <row r="299" spans="18:20" x14ac:dyDescent="0.3">
       <c r="R299">
         <v>0.39146068581955712</v>
       </c>
@@ -24739,7 +24730,7 @@
         <v>1.5986349565829481</v>
       </c>
     </row>
-    <row r="300" spans="18:20" x14ac:dyDescent="0.25">
+    <row r="300" spans="18:20" x14ac:dyDescent="0.3">
       <c r="R300">
         <v>0.39267353297672125</v>
       </c>
@@ -24750,7 +24741,7 @@
         <v>1.6030488503726068</v>
       </c>
     </row>
-    <row r="301" spans="18:20" x14ac:dyDescent="0.25">
+    <row r="301" spans="18:20" x14ac:dyDescent="0.3">
       <c r="R301">
         <v>0.39388638013388538</v>
       </c>
@@ -24761,7 +24752,7 @@
         <v>1.6074502026204764</v>
       </c>
     </row>
-    <row r="302" spans="18:20" x14ac:dyDescent="0.25">
+    <row r="302" spans="18:20" x14ac:dyDescent="0.3">
       <c r="R302">
         <v>0.39527891088824169</v>
       </c>
@@ -24772,7 +24763,7 @@
         <v>1.612484020563695</v>
       </c>
     </row>
-    <row r="303" spans="18:20" x14ac:dyDescent="0.25">
+    <row r="303" spans="18:20" x14ac:dyDescent="0.3">
       <c r="R303">
         <v>0.39667144164259799</v>
       </c>
@@ -24783,7 +24774,7 @@
         <v>1.6175010529004634</v>
       </c>
     </row>
-    <row r="304" spans="18:20" x14ac:dyDescent="0.25">
+    <row r="304" spans="18:20" x14ac:dyDescent="0.3">
       <c r="R304">
         <v>0.39806397239695429</v>
       </c>
@@ -24794,7 +24785,7 @@
         <v>1.6225017449542278</v>
       </c>
     </row>
-    <row r="305" spans="18:20" x14ac:dyDescent="0.25">
+    <row r="305" spans="18:20" x14ac:dyDescent="0.3">
       <c r="R305">
         <v>0.4</v>
       </c>
@@ -24805,7 +24796,7 @@
         <v>1.6294314249371693</v>
       </c>
     </row>
-    <row r="306" spans="18:20" x14ac:dyDescent="0.25">
+    <row r="306" spans="18:20" x14ac:dyDescent="0.3">
       <c r="R306">
         <v>0.40193602760304575</v>
       </c>
@@ -24816,7 +24807,7 @@
         <v>1.6363318329989478</v>
       </c>
     </row>
-    <row r="307" spans="18:20" x14ac:dyDescent="0.25">
+    <row r="307" spans="18:20" x14ac:dyDescent="0.3">
       <c r="R307">
         <v>0.40387205520609148</v>
       </c>
@@ -24827,7 +24818,7 @@
         <v>1.6432016028083987</v>
       </c>
     </row>
-    <row r="308" spans="18:20" x14ac:dyDescent="0.25">
+    <row r="308" spans="18:20" x14ac:dyDescent="0.3">
       <c r="R308">
         <v>0.40580808280913722</v>
       </c>
@@ -24838,7 +24829,7 @@
         <v>1.650040441777771</v>
       </c>
     </row>
-    <row r="309" spans="18:20" x14ac:dyDescent="0.25">
+    <row r="309" spans="18:20" x14ac:dyDescent="0.3">
       <c r="R309">
         <v>0.4074297859336653</v>
       </c>
@@ -24849,7 +24840,7 @@
         <v>1.6557453351045921</v>
       </c>
     </row>
-    <row r="310" spans="18:20" x14ac:dyDescent="0.25">
+    <row r="310" spans="18:20" x14ac:dyDescent="0.3">
       <c r="R310">
         <v>0.40905148905819338</v>
       </c>
@@ -24860,7 +24851,7 @@
         <v>1.661430643118754</v>
       </c>
     </row>
-    <row r="311" spans="18:20" x14ac:dyDescent="0.25">
+    <row r="311" spans="18:20" x14ac:dyDescent="0.3">
       <c r="R311">
         <v>0.41067319218272147</v>
       </c>
@@ -24871,7 +24862,7 @@
         <v>1.6670979611915677</v>
       </c>
     </row>
-    <row r="312" spans="18:20" x14ac:dyDescent="0.25">
+    <row r="312" spans="18:20" x14ac:dyDescent="0.3">
       <c r="R312">
         <v>0.41229489530724955</v>
       </c>
@@ -24882,7 +24873,7 @@
         <v>1.6727476925408635</v>
       </c>
     </row>
-    <row r="313" spans="18:20" x14ac:dyDescent="0.25">
+    <row r="313" spans="18:20" x14ac:dyDescent="0.3">
       <c r="R313">
         <v>0.41576453527167995</v>
       </c>
@@ -24893,7 +24884,7 @@
         <v>1.6847506129505341</v>
       </c>
     </row>
-    <row r="314" spans="18:20" x14ac:dyDescent="0.25">
+    <row r="314" spans="18:20" x14ac:dyDescent="0.3">
       <c r="R314">
         <v>0.41923417523611034</v>
       </c>
@@ -24904,7 +24895,7 @@
         <v>1.6966717103737992</v>
       </c>
     </row>
-    <row r="315" spans="18:20" x14ac:dyDescent="0.25">
+    <row r="315" spans="18:20" x14ac:dyDescent="0.3">
       <c r="R315">
         <v>0.42</v>
       </c>
@@ -24915,7 +24906,7 @@
         <v>1.6992967832598782</v>
       </c>
     </row>
-    <row r="316" spans="18:20" x14ac:dyDescent="0.25">
+    <row r="316" spans="18:20" x14ac:dyDescent="0.3">
       <c r="R316">
         <v>0.42076582476388963</v>
       </c>
@@ -24926,7 +24917,7 @@
         <v>1.7019175423972377</v>
       </c>
     </row>
-    <row r="317" spans="18:20" x14ac:dyDescent="0.25">
+    <row r="317" spans="18:20" x14ac:dyDescent="0.3">
       <c r="R317">
         <v>0.42153164952777927</v>
       </c>
@@ -24937,7 +24928,7 @@
         <v>1.7045342866008828</v>
       </c>
     </row>
-    <row r="318" spans="18:20" x14ac:dyDescent="0.25">
+    <row r="318" spans="18:20" x14ac:dyDescent="0.3">
       <c r="R318">
         <v>0.42647671460999637</v>
       </c>
@@ -24948,7 +24939,7 @@
         <v>1.721294159720439</v>
       </c>
     </row>
-    <row r="319" spans="18:20" x14ac:dyDescent="0.25">
+    <row r="319" spans="18:20" x14ac:dyDescent="0.3">
       <c r="R319">
         <v>0.43142177969221346</v>
       </c>
@@ -24959,7 +24950,7 @@
         <v>1.737906309046287</v>
       </c>
     </row>
-    <row r="320" spans="18:20" x14ac:dyDescent="0.25">
+    <row r="320" spans="18:20" x14ac:dyDescent="0.3">
       <c r="R320">
         <v>0.43245133983837197</v>
       </c>
@@ -24970,7 +24961,7 @@
         <v>1.7413547055143082</v>
       </c>
     </row>
-    <row r="321" spans="18:20" x14ac:dyDescent="0.25">
+    <row r="321" spans="18:20" x14ac:dyDescent="0.3">
       <c r="R321">
         <v>0.43267146538091611</v>
       </c>
@@ -24981,7 +24972,7 @@
         <v>1.7420917792030375</v>
       </c>
     </row>
-    <row r="322" spans="18:20" x14ac:dyDescent="0.25">
+    <row r="322" spans="18:20" x14ac:dyDescent="0.3">
       <c r="R322">
         <v>0.43289159092346025</v>
       </c>
@@ -24992,7 +24983,7 @@
         <v>1.7428292475443619</v>
       </c>
     </row>
-    <row r="323" spans="18:20" x14ac:dyDescent="0.25">
+    <row r="323" spans="18:20" x14ac:dyDescent="0.3">
       <c r="R323">
         <v>0.43311171646600438</v>
       </c>
@@ -25003,7 +24994,7 @@
         <v>1.7435672364896249</v>
       </c>
     </row>
-    <row r="324" spans="18:20" x14ac:dyDescent="0.25">
+    <row r="324" spans="18:20" x14ac:dyDescent="0.3">
       <c r="R324">
         <v>0.43411557244476978</v>
       </c>
@@ -25014,7 +25005,7 @@
         <v>1.7469411988423937</v>
       </c>
     </row>
-    <row r="325" spans="18:20" x14ac:dyDescent="0.25">
+    <row r="325" spans="18:20" x14ac:dyDescent="0.3">
       <c r="R325">
         <v>0.43511942842353518</v>
       </c>
@@ -25025,7 +25016,7 @@
         <v>1.7503228367737997</v>
       </c>
     </row>
-    <row r="326" spans="18:20" x14ac:dyDescent="0.25">
+    <row r="326" spans="18:20" x14ac:dyDescent="0.3">
       <c r="R326">
         <v>0.43612328440230058</v>
       </c>
@@ -25036,7 +25027,7 @@
         <v>1.7537103412605131</v>
       </c>
     </row>
-    <row r="327" spans="18:20" x14ac:dyDescent="0.25">
+    <row r="327" spans="18:20" x14ac:dyDescent="0.3">
       <c r="R327">
         <v>0.43800908605567418</v>
       </c>
@@ -25047,7 +25038,7 @@
         <v>1.7600822744663085</v>
       </c>
     </row>
-    <row r="328" spans="18:20" x14ac:dyDescent="0.25">
+    <row r="328" spans="18:20" x14ac:dyDescent="0.3">
       <c r="R328">
         <v>0.44</v>
       </c>
@@ -25058,7 +25049,7 @@
         <v>1.7668148457586281</v>
       </c>
     </row>
-    <row r="329" spans="18:20" x14ac:dyDescent="0.25">
+    <row r="329" spans="18:20" x14ac:dyDescent="0.3">
       <c r="R329">
         <v>0.44199091394432583</v>
       </c>
@@ -25069,7 +25060,7 @@
         <v>1.7735435073093999</v>
       </c>
     </row>
-    <row r="330" spans="18:20" x14ac:dyDescent="0.25">
+    <row r="330" spans="18:20" x14ac:dyDescent="0.3">
       <c r="R330">
         <v>0.44398182788865165</v>
       </c>
@@ -25080,7 +25071,7 @@
         <v>1.7802591774428156</v>
       </c>
     </row>
-    <row r="331" spans="18:20" x14ac:dyDescent="0.25">
+    <row r="331" spans="18:20" x14ac:dyDescent="0.3">
       <c r="R331">
         <v>0.44597274183297747</v>
       </c>
@@ -25091,7 +25082,7 @@
         <v>1.7869542627830182</v>
       </c>
     </row>
-    <row r="332" spans="18:20" x14ac:dyDescent="0.25">
+    <row r="332" spans="18:20" x14ac:dyDescent="0.3">
       <c r="R332">
         <v>0.4493768779920525</v>
       </c>
@@ -25102,7 +25093,7 @@
         <v>1.7983389989135072</v>
       </c>
     </row>
-    <row r="333" spans="18:20" x14ac:dyDescent="0.25">
+    <row r="333" spans="18:20" x14ac:dyDescent="0.3">
       <c r="R333">
         <v>0.45278101415112754</v>
       </c>
@@ -25113,7 +25104,7 @@
         <v>1.8096258852277591</v>
       </c>
     </row>
-    <row r="334" spans="18:20" x14ac:dyDescent="0.25">
+    <row r="334" spans="18:20" x14ac:dyDescent="0.3">
       <c r="R334">
         <v>0.45380225499885007</v>
       </c>
@@ -25124,7 +25115,7 @@
         <v>1.8129903497403359</v>
       </c>
     </row>
-    <row r="335" spans="18:20" x14ac:dyDescent="0.25">
+    <row r="335" spans="18:20" x14ac:dyDescent="0.3">
       <c r="R335">
         <v>0.45482349584657261</v>
       </c>
@@ -25135,7 +25126,7 @@
         <v>1.8163446728503851</v>
       </c>
     </row>
-    <row r="336" spans="18:20" x14ac:dyDescent="0.25">
+    <row r="336" spans="18:20" x14ac:dyDescent="0.3">
       <c r="R336">
         <v>0.45584473669429515</v>
       </c>
@@ -25146,7 +25137,7 @@
         <v>1.8196882331000843</v>
       </c>
     </row>
-    <row r="337" spans="18:20" x14ac:dyDescent="0.25">
+    <row r="337" spans="18:20" x14ac:dyDescent="0.3">
       <c r="R337">
         <v>0.45686597754201769</v>
       </c>
@@ -25157,7 +25148,7 @@
         <v>1.8230208634265193</v>
       </c>
     </row>
-    <row r="338" spans="18:20" x14ac:dyDescent="0.25">
+    <row r="338" spans="18:20" x14ac:dyDescent="0.3">
       <c r="R338">
         <v>0.45788721838974022</v>
       </c>
@@ -25168,7 +25159,7 @@
         <v>1.8263426691659106</v>
       </c>
     </row>
-    <row r="339" spans="18:20" x14ac:dyDescent="0.25">
+    <row r="339" spans="18:20" x14ac:dyDescent="0.3">
       <c r="R339">
         <v>0.46</v>
       </c>
@@ -25179,7 +25170,7 @@
         <v>1.8331813545765758</v>
       </c>
     </row>
-    <row r="340" spans="18:20" x14ac:dyDescent="0.25">
+    <row r="340" spans="18:20" x14ac:dyDescent="0.3">
       <c r="R340">
         <v>0.46211278161025982</v>
       </c>
@@ -25190,7 +25181,7 @@
         <v>1.8399756077680873</v>
       </c>
     </row>
-    <row r="341" spans="18:20" x14ac:dyDescent="0.25">
+    <row r="341" spans="18:20" x14ac:dyDescent="0.3">
       <c r="R341">
         <v>0.46422556322051961</v>
       </c>
@@ -25201,7 +25192,7 @@
         <v>1.8467271744089611</v>
       </c>
     </row>
-    <row r="342" spans="18:20" x14ac:dyDescent="0.25">
+    <row r="342" spans="18:20" x14ac:dyDescent="0.3">
       <c r="R342">
         <v>0.46633834483077941</v>
       </c>
@@ -25212,7 +25203,7 @@
         <v>1.8534379960496383</v>
       </c>
     </row>
-    <row r="343" spans="18:20" x14ac:dyDescent="0.25">
+    <row r="343" spans="18:20" x14ac:dyDescent="0.3">
       <c r="R343">
         <v>0.47223939673460658</v>
       </c>
@@ -25223,7 +25214,7 @@
         <v>1.8719914290361119</v>
       </c>
     </row>
-    <row r="344" spans="18:20" x14ac:dyDescent="0.25">
+    <row r="344" spans="18:20" x14ac:dyDescent="0.3">
       <c r="R344">
         <v>0.47814044863843375</v>
       </c>
@@ -25234,7 +25225,7 @@
         <v>1.8902948856571791</v>
       </c>
     </row>
-    <row r="345" spans="18:20" x14ac:dyDescent="0.25">
+    <row r="345" spans="18:20" x14ac:dyDescent="0.3">
       <c r="R345">
         <v>0.48</v>
       </c>
@@ -25245,7 +25236,7 @@
         <v>1.8960155622102093</v>
       </c>
     </row>
-    <row r="346" spans="18:20" x14ac:dyDescent="0.25">
+    <row r="346" spans="18:20" x14ac:dyDescent="0.3">
       <c r="R346">
         <v>0.48185955136156622</v>
       </c>
@@ -25256,7 +25247,7 @@
         <v>1.9017179076800499</v>
       </c>
     </row>
-    <row r="347" spans="18:20" x14ac:dyDescent="0.25">
+    <row r="347" spans="18:20" x14ac:dyDescent="0.3">
       <c r="R347">
         <v>0.48371910272313245</v>
       </c>
@@ -25267,7 +25258,7 @@
         <v>1.9074031518973578</v>
       </c>
     </row>
-    <row r="348" spans="18:20" x14ac:dyDescent="0.25">
+    <row r="348" spans="18:20" x14ac:dyDescent="0.3">
       <c r="R348">
         <v>0.48557865408469869</v>
       </c>
@@ -25278,7 +25269,7 @@
         <v>1.9130724337290759</v>
       </c>
     </row>
-    <row r="349" spans="18:20" x14ac:dyDescent="0.25">
+    <row r="349" spans="18:20" x14ac:dyDescent="0.3">
       <c r="R349">
         <v>0.49456160206021327</v>
       </c>
@@ -25289,7 +25280,7 @@
         <v>1.9402754026268556</v>
       </c>
     </row>
-    <row r="350" spans="18:20" x14ac:dyDescent="0.25">
+    <row r="350" spans="18:20" x14ac:dyDescent="0.3">
       <c r="R350">
         <v>0.49619312144214928</v>
       </c>
@@ -25300,7 +25291,7 @@
         <v>1.9451838835232893</v>
       </c>
     </row>
-    <row r="351" spans="18:20" x14ac:dyDescent="0.25">
+    <row r="351" spans="18:20" x14ac:dyDescent="0.3">
       <c r="R351">
         <v>0.49667475729992561</v>
       </c>
@@ -25311,7 +25302,7 @@
         <v>1.9466325631408741</v>
       </c>
     </row>
-    <row r="352" spans="18:20" x14ac:dyDescent="0.25">
+    <row r="352" spans="18:20" x14ac:dyDescent="0.3">
       <c r="R352">
         <v>0.49715639315770194</v>
       </c>
@@ -25322,7 +25313,7 @@
         <v>1.9480831582436071</v>
       </c>
     </row>
-    <row r="353" spans="18:20" x14ac:dyDescent="0.25">
+    <row r="353" spans="18:20" x14ac:dyDescent="0.3">
       <c r="R353">
         <v>0.49763802901547827</v>
       </c>
@@ -25333,7 +25324,7 @@
         <v>1.9495353748438644</v>
       </c>
     </row>
-    <row r="354" spans="18:20" x14ac:dyDescent="0.25">
+    <row r="354" spans="18:20" x14ac:dyDescent="0.3">
       <c r="R354">
         <v>0.4981196648732546</v>
       </c>
@@ -25344,7 +25335,7 @@
         <v>1.9509886883776275</v>
       </c>
     </row>
-    <row r="355" spans="18:20" x14ac:dyDescent="0.25">
+    <row r="355" spans="18:20" x14ac:dyDescent="0.3">
       <c r="R355">
         <v>0.49963191284200004</v>
       </c>
@@ -25355,7 +25346,7 @@
         <v>1.9555582079735201</v>
       </c>
     </row>
-    <row r="356" spans="18:20" x14ac:dyDescent="0.25">
+    <row r="356" spans="18:20" x14ac:dyDescent="0.3">
       <c r="R356">
         <v>0.5</v>
       </c>
@@ -25366,7 +25357,7 @@
         <v>1.9566709618320548</v>
       </c>
     </row>
-    <row r="357" spans="18:20" x14ac:dyDescent="0.25">
+    <row r="357" spans="18:20" x14ac:dyDescent="0.3">
       <c r="R357">
         <v>0.50036808715799996</v>
       </c>
@@ -25377,7 +25368,7 @@
         <v>1.9577840229960279</v>
       </c>
     </row>
-    <row r="358" spans="18:20" x14ac:dyDescent="0.25">
+    <row r="358" spans="18:20" x14ac:dyDescent="0.3">
       <c r="R358">
         <v>0.50073617431599993</v>
       </c>
@@ -25388,7 +25379,7 @@
         <v>1.9588973286044</v>
       </c>
     </row>
-    <row r="359" spans="18:20" x14ac:dyDescent="0.25">
+    <row r="359" spans="18:20" x14ac:dyDescent="0.3">
       <c r="R359">
         <v>0.50256445865524613</v>
       </c>
@@ -25399,7 +25390,7 @@
         <v>1.9644292378948958</v>
       </c>
     </row>
-    <row r="360" spans="18:20" x14ac:dyDescent="0.25">
+    <row r="360" spans="18:20" x14ac:dyDescent="0.3">
       <c r="R360">
         <v>0.50439274299449233</v>
       </c>
@@ -25410,7 +25401,7 @@
         <v>1.9699603887100579</v>
       </c>
     </row>
-    <row r="361" spans="18:20" x14ac:dyDescent="0.25">
+    <row r="361" spans="18:20" x14ac:dyDescent="0.3">
       <c r="R361">
         <v>0.50622102733373853</v>
       </c>
@@ -25421,7 +25412,7 @@
         <v>1.9754875715763158</v>
       </c>
     </row>
-    <row r="362" spans="18:20" x14ac:dyDescent="0.25">
+    <row r="362" spans="18:20" x14ac:dyDescent="0.3">
       <c r="R362">
         <v>0.51013808904024405</v>
       </c>
@@ -25432,7 +25423,7 @@
         <v>1.9873054456342216</v>
       </c>
     </row>
-    <row r="363" spans="18:20" x14ac:dyDescent="0.25">
+    <row r="363" spans="18:20" x14ac:dyDescent="0.3">
       <c r="R363">
         <v>0.51405515074674957</v>
       </c>
@@ -25443,7 +25434,7 @@
         <v>1.9990745112662283</v>
       </c>
     </row>
-    <row r="364" spans="18:20" x14ac:dyDescent="0.25">
+    <row r="364" spans="18:20" x14ac:dyDescent="0.3">
       <c r="R364">
         <v>0.51797221245325509</v>
       </c>
@@ -25454,7 +25445,7 @@
         <v>2.0107760871202469</v>
       </c>
     </row>
-    <row r="365" spans="18:20" x14ac:dyDescent="0.25">
+    <row r="365" spans="18:20" x14ac:dyDescent="0.3">
       <c r="R365">
         <v>0.52</v>
       </c>
@@ -25465,7 +25456,7 @@
         <v>2.0168032690505813</v>
       </c>
     </row>
-    <row r="366" spans="18:20" x14ac:dyDescent="0.25">
+    <row r="366" spans="18:20" x14ac:dyDescent="0.3">
       <c r="R366">
         <v>0.52202778754674495</v>
       </c>
@@ -25476,7 +25467,7 @@
         <v>2.0228066784389989</v>
       </c>
     </row>
-    <row r="367" spans="18:20" x14ac:dyDescent="0.25">
+    <row r="367" spans="18:20" x14ac:dyDescent="0.3">
       <c r="R367">
         <v>0.52405557509348988</v>
       </c>
@@ -25487,7 +25478,7 @@
         <v>2.0287853757423742</v>
       </c>
     </row>
-    <row r="368" spans="18:20" x14ac:dyDescent="0.25">
+    <row r="368" spans="18:20" x14ac:dyDescent="0.3">
       <c r="R368">
         <v>0.52608336264023481</v>
       </c>
@@ -25498,7 +25489,7 @@
         <v>2.0347387277138207</v>
       </c>
     </row>
-    <row r="369" spans="18:20" x14ac:dyDescent="0.25">
+    <row r="369" spans="18:20" x14ac:dyDescent="0.3">
       <c r="R369">
         <v>0.53311368024066563</v>
       </c>
@@ -25509,7 +25500,7 @@
         <v>2.0551798818693738</v>
       </c>
     </row>
-    <row r="370" spans="18:20" x14ac:dyDescent="0.25">
+    <row r="370" spans="18:20" x14ac:dyDescent="0.3">
       <c r="R370">
         <v>0.54</v>
       </c>
@@ -25520,7 +25511,7 @@
         <v>2.0749015530018431</v>
       </c>
     </row>
-    <row r="371" spans="18:20" x14ac:dyDescent="0.25">
+    <row r="371" spans="18:20" x14ac:dyDescent="0.3">
       <c r="R371">
         <v>0.54688631975933444</v>
       </c>
@@ -25531,7 +25522,7 @@
         <v>2.0943380627586539</v>
       </c>
     </row>
-    <row r="372" spans="18:20" x14ac:dyDescent="0.25">
+    <row r="372" spans="18:20" x14ac:dyDescent="0.3">
       <c r="R372">
         <v>0.54836044501633474</v>
       </c>
@@ -25542,7 +25533,7 @@
         <v>2.0984634493848668</v>
       </c>
     </row>
-    <row r="373" spans="18:20" x14ac:dyDescent="0.25">
+    <row r="373" spans="18:20" x14ac:dyDescent="0.3">
       <c r="R373">
         <v>0.54856826848824902</v>
       </c>
@@ -25553,7 +25544,7 @@
         <v>2.0990441370271018</v>
       </c>
     </row>
-    <row r="374" spans="18:20" x14ac:dyDescent="0.25">
+    <row r="374" spans="18:20" x14ac:dyDescent="0.3">
       <c r="R374">
         <v>0.54874576029491351</v>
       </c>
@@ -25564,7 +25555,7 @@
         <v>2.0995400083234816</v>
       </c>
     </row>
-    <row r="375" spans="18:20" x14ac:dyDescent="0.25">
+    <row r="375" spans="18:20" x14ac:dyDescent="0.3">
       <c r="R375">
         <v>0.548923252101578</v>
       </c>
@@ -25575,7 +25566,7 @@
         <v>2.1000359579486796</v>
       </c>
     </row>
-    <row r="376" spans="18:20" x14ac:dyDescent="0.25">
+    <row r="376" spans="18:20" x14ac:dyDescent="0.3">
       <c r="R376">
         <v>0.54910074390824248</v>
       </c>
@@ -25586,7 +25577,7 @@
         <v>2.1005320735450757</v>
       </c>
     </row>
-    <row r="377" spans="18:20" x14ac:dyDescent="0.25">
+    <row r="377" spans="18:20" x14ac:dyDescent="0.3">
       <c r="R377">
         <v>0.54927823571490697</v>
       </c>
@@ -25597,7 +25588,7 @@
         <v>2.1010283938321046</v>
       </c>
     </row>
-    <row r="378" spans="18:20" x14ac:dyDescent="0.25">
+    <row r="378" spans="18:20" x14ac:dyDescent="0.3">
       <c r="R378">
         <v>0.55020361465304402</v>
       </c>
@@ -25608,7 +25599,7 @@
         <v>2.1036208590702188</v>
       </c>
     </row>
-    <row r="379" spans="18:20" x14ac:dyDescent="0.25">
+    <row r="379" spans="18:20" x14ac:dyDescent="0.3">
       <c r="R379">
         <v>0.55112899359118106</v>
       </c>
@@ -25619,7 +25610,7 @@
         <v>2.1062176375775326</v>
       </c>
     </row>
-    <row r="380" spans="18:20" x14ac:dyDescent="0.25">
+    <row r="380" spans="18:20" x14ac:dyDescent="0.3">
       <c r="R380">
         <v>0.5520543725293181</v>
       </c>
@@ -25630,7 +25621,7 @@
         <v>2.1088178540072362</v>
       </c>
     </row>
-    <row r="381" spans="18:20" x14ac:dyDescent="0.25">
+    <row r="381" spans="18:20" x14ac:dyDescent="0.3">
       <c r="R381">
         <v>0.55263898034285064</v>
       </c>
@@ -25641,7 +25632,7 @@
         <v>2.1104617227646276</v>
       </c>
     </row>
-    <row r="382" spans="18:20" x14ac:dyDescent="0.25">
+    <row r="382" spans="18:20" x14ac:dyDescent="0.3">
       <c r="R382">
         <v>0.55284102277477698</v>
       </c>
@@ -25652,7 +25643,7 @@
         <v>2.1110302875174765</v>
       </c>
     </row>
-    <row r="383" spans="18:20" x14ac:dyDescent="0.25">
+    <row r="383" spans="18:20" x14ac:dyDescent="0.3">
       <c r="R383">
         <v>0.55304306520670332</v>
       </c>
@@ -25663,7 +25654,7 @@
         <v>2.1115993197862393</v>
       </c>
     </row>
-    <row r="384" spans="18:20" x14ac:dyDescent="0.25">
+    <row r="384" spans="18:20" x14ac:dyDescent="0.3">
       <c r="R384">
         <v>0.55324510763862966</v>
       </c>
@@ -25674,7 +25665,7 @@
         <v>2.1121687906038984</v>
       </c>
     </row>
-    <row r="385" spans="18:20" x14ac:dyDescent="0.25">
+    <row r="385" spans="18:20" x14ac:dyDescent="0.3">
       <c r="R385">
         <v>0.553447150070556</v>
       </c>
@@ -25685,7 +25676,7 @@
         <v>2.1127386430295667</v>
       </c>
     </row>
-    <row r="386" spans="18:20" x14ac:dyDescent="0.25">
+    <row r="386" spans="18:20" x14ac:dyDescent="0.3">
       <c r="R386">
         <v>0.55427541273383629</v>
       </c>
@@ -25696,7 +25687,7 @@
         <v>2.1150793455243679</v>
       </c>
     </row>
-    <row r="387" spans="18:20" x14ac:dyDescent="0.25">
+    <row r="387" spans="18:20" x14ac:dyDescent="0.3">
       <c r="R387">
         <v>0.55510367539711658</v>
       </c>
@@ -25707,7 +25698,7 @@
         <v>2.1174241749871952</v>
       </c>
     </row>
-    <row r="388" spans="18:20" x14ac:dyDescent="0.25">
+    <row r="388" spans="18:20" x14ac:dyDescent="0.3">
       <c r="R388">
         <v>0.55593193806039687</v>
       </c>
@@ -25718,7 +25709,7 @@
         <v>2.1197722217923283</v>
       </c>
     </row>
-    <row r="389" spans="18:20" x14ac:dyDescent="0.25">
+    <row r="389" spans="18:20" x14ac:dyDescent="0.3">
       <c r="R389">
         <v>0.55705585042096339</v>
       </c>
@@ -25729,7 +25720,7 @@
         <v>2.1229615504376969</v>
       </c>
     </row>
-    <row r="390" spans="18:20" x14ac:dyDescent="0.25">
+    <row r="390" spans="18:20" x14ac:dyDescent="0.3">
       <c r="R390">
         <v>0.55817976278152992</v>
       </c>
@@ -25740,7 +25731,7 @@
         <v>2.1261534621954317</v>
       </c>
     </row>
-    <row r="391" spans="18:20" x14ac:dyDescent="0.25">
+    <row r="391" spans="18:20" x14ac:dyDescent="0.3">
       <c r="R391">
         <v>0.55930367514209645</v>
       </c>
@@ -25751,7 +25742,7 @@
         <v>2.1293463311440854</v>
       </c>
     </row>
-    <row r="392" spans="18:20" x14ac:dyDescent="0.25">
+    <row r="392" spans="18:20" x14ac:dyDescent="0.3">
       <c r="R392">
         <v>0.56000000000000005</v>
       </c>
@@ -25762,7 +25753,7 @@
         <v>2.1313243238777044</v>
       </c>
     </row>
-    <row r="393" spans="18:20" x14ac:dyDescent="0.25">
+    <row r="393" spans="18:20" x14ac:dyDescent="0.3">
       <c r="R393">
         <v>0.56069632485790366</v>
       </c>
@@ -25773,7 +25764,7 @@
         <v>2.1333015749689466</v>
       </c>
     </row>
-    <row r="394" spans="18:20" x14ac:dyDescent="0.25">
+    <row r="394" spans="18:20" x14ac:dyDescent="0.3">
       <c r="R394">
         <v>0.56139264971580727</v>
       </c>
@@ -25784,7 +25775,7 @@
         <v>2.1352776847532713</v>
       </c>
     </row>
-    <row r="395" spans="18:20" x14ac:dyDescent="0.25">
+    <row r="395" spans="18:20" x14ac:dyDescent="0.3">
       <c r="R395">
         <v>0.56208897457371088</v>
       </c>
@@ -25795,7 +25786,7 @@
         <v>2.137252280102544</v>
       </c>
     </row>
-    <row r="396" spans="18:20" x14ac:dyDescent="0.25">
+    <row r="396" spans="18:20" x14ac:dyDescent="0.3">
       <c r="R396">
         <v>0.56525202828553334</v>
       </c>
@@ -25806,7 +25797,7 @@
         <v>2.1461899444632531</v>
       </c>
     </row>
-    <row r="397" spans="18:20" x14ac:dyDescent="0.25">
+    <row r="397" spans="18:20" x14ac:dyDescent="0.3">
       <c r="R397">
         <v>0.5684150819973558</v>
       </c>
@@ -25817,7 +25808,7 @@
         <v>2.1550625452566528</v>
       </c>
     </row>
-    <row r="398" spans="18:20" x14ac:dyDescent="0.25">
+    <row r="398" spans="18:20" x14ac:dyDescent="0.3">
       <c r="R398">
         <v>0.57157813570917826</v>
       </c>
@@ -25828,7 +25819,7 @@
         <v>2.1638503475685216</v>
       </c>
     </row>
-    <row r="399" spans="18:20" x14ac:dyDescent="0.25">
+    <row r="399" spans="18:20" x14ac:dyDescent="0.3">
       <c r="R399">
         <v>0.57474118942100072</v>
       </c>
@@ -25839,7 +25830,7 @@
         <v>2.1725388288638245</v>
       </c>
     </row>
-    <row r="400" spans="18:20" x14ac:dyDescent="0.25">
+    <row r="400" spans="18:20" x14ac:dyDescent="0.3">
       <c r="R400">
         <v>0.57950362845660752</v>
       </c>
@@ -25850,7 +25841,7 @@
         <v>2.1854170076987356</v>
       </c>
     </row>
-    <row r="401" spans="18:20" x14ac:dyDescent="0.25">
+    <row r="401" spans="18:20" x14ac:dyDescent="0.3">
       <c r="R401">
         <v>0.57999999999999996</v>
       </c>
@@ -25861,7 +25852,7 @@
         <v>2.1867441848257831</v>
       </c>
     </row>
-    <row r="402" spans="18:20" x14ac:dyDescent="0.25">
+    <row r="402" spans="18:20" x14ac:dyDescent="0.3">
       <c r="R402">
         <v>0.5804963715433924</v>
       </c>
@@ -25872,7 +25863,7 @@
         <v>2.1880686560705516</v>
       </c>
     </row>
-    <row r="403" spans="18:20" x14ac:dyDescent="0.25">
+    <row r="403" spans="18:20" x14ac:dyDescent="0.3">
       <c r="R403">
         <v>0.58099274308678484</v>
       </c>
@@ -25883,7 +25874,7 @@
         <v>2.1893903856073633</v>
       </c>
     </row>
-    <row r="404" spans="18:20" x14ac:dyDescent="0.25">
+    <row r="404" spans="18:20" x14ac:dyDescent="0.3">
       <c r="R404">
         <v>0.58148911463017727</v>
       </c>
@@ -25894,7 +25885,7 @@
         <v>2.1907093436081144</v>
       </c>
     </row>
-    <row r="405" spans="18:20" x14ac:dyDescent="0.25">
+    <row r="405" spans="18:20" x14ac:dyDescent="0.3">
       <c r="R405">
         <v>0.58198548617356971</v>
       </c>
@@ -25905,7 +25896,7 @@
         <v>2.1920255296284683</v>
       </c>
     </row>
-    <row r="406" spans="18:20" x14ac:dyDescent="0.25">
+    <row r="406" spans="18:20" x14ac:dyDescent="0.3">
       <c r="R406">
         <v>0.58625369054646537</v>
       </c>
@@ -25916,7 +25907,7 @@
         <v>2.2032335159513314</v>
       </c>
     </row>
-    <row r="407" spans="18:20" x14ac:dyDescent="0.25">
+    <row r="407" spans="18:20" x14ac:dyDescent="0.3">
       <c r="R407">
         <v>0.59052189491936102</v>
       </c>
@@ -25927,7 +25918,7 @@
         <v>2.2142526852118505</v>
       </c>
     </row>
-    <row r="408" spans="18:20" x14ac:dyDescent="0.25">
+    <row r="408" spans="18:20" x14ac:dyDescent="0.3">
       <c r="R408">
         <v>0.59479009929225668</v>
       </c>
@@ -25938,7 +25929,7 @@
         <v>2.225099718827908</v>
       </c>
     </row>
-    <row r="409" spans="18:20" x14ac:dyDescent="0.25">
+    <row r="409" spans="18:20" x14ac:dyDescent="0.3">
       <c r="R409">
         <v>0.59905830366515234</v>
       </c>
@@ -25949,7 +25940,7 @@
         <v>2.2357944489549424</v>
       </c>
     </row>
-    <row r="410" spans="18:20" x14ac:dyDescent="0.25">
+    <row r="410" spans="18:20" x14ac:dyDescent="0.3">
       <c r="R410">
         <v>0.6</v>
       </c>
@@ -25960,7 +25951,7 @@
         <v>2.2381351780547933</v>
       </c>
     </row>
-    <row r="411" spans="18:20" x14ac:dyDescent="0.25">
+    <row r="411" spans="18:20" x14ac:dyDescent="0.3">
       <c r="R411">
         <v>0.60094169633484762</v>
       </c>
@@ -25971,7 +25962,7 @@
         <v>2.2404694556258371</v>
       </c>
     </row>
-    <row r="412" spans="18:20" x14ac:dyDescent="0.25">
+    <row r="412" spans="18:20" x14ac:dyDescent="0.3">
       <c r="R412">
         <v>0.60188339266969526</v>
       </c>
@@ -25982,7 +25973,7 @@
         <v>2.2427977148257776</v>
       </c>
     </row>
-    <row r="413" spans="18:20" x14ac:dyDescent="0.25">
+    <row r="413" spans="18:20" x14ac:dyDescent="0.3">
       <c r="R413">
         <v>0.6028250890045429</v>
       </c>
@@ -25993,7 +25984,7 @@
         <v>2.2451202841504747</v>
       </c>
     </row>
-    <row r="414" spans="18:20" x14ac:dyDescent="0.25">
+    <row r="414" spans="18:20" x14ac:dyDescent="0.3">
       <c r="R414">
         <v>0.60376678533939054</v>
       </c>
@@ -26004,7 +25995,7 @@
         <v>2.2474373922108395</v>
       </c>
     </row>
-    <row r="415" spans="18:20" x14ac:dyDescent="0.25">
+    <row r="415" spans="18:20" x14ac:dyDescent="0.3">
       <c r="R415">
         <v>0.60920012993109396</v>
       </c>
@@ -26015,7 +26006,7 @@
         <v>2.2607141090352352</v>
       </c>
     </row>
-    <row r="416" spans="18:20" x14ac:dyDescent="0.25">
+    <row r="416" spans="18:20" x14ac:dyDescent="0.3">
       <c r="R416">
         <v>0.61463347452279737</v>
       </c>
@@ -26026,7 +26017,7 @@
         <v>2.2738485335161642</v>
       </c>
     </row>
-    <row r="417" spans="18:20" x14ac:dyDescent="0.25">
+    <row r="417" spans="18:20" x14ac:dyDescent="0.3">
       <c r="R417">
         <v>0.62</v>
       </c>
@@ -26037,7 +26028,7 @@
         <v>2.2867053294227833</v>
       </c>
     </row>
-    <row r="418" spans="18:20" x14ac:dyDescent="0.25">
+    <row r="418" spans="18:20" x14ac:dyDescent="0.3">
       <c r="R418">
         <v>0.62536652547720262</v>
       </c>
@@ -26048,7 +26039,7 @@
         <v>2.2994633562225193</v>
       </c>
     </row>
-    <row r="419" spans="18:20" x14ac:dyDescent="0.25">
+    <row r="419" spans="18:20" x14ac:dyDescent="0.3">
       <c r="R419">
         <v>0.63073305095440524</v>
       </c>
@@ -26059,7 +26050,7 @@
         <v>2.3121308332600727</v>
       </c>
     </row>
-    <row r="420" spans="18:20" x14ac:dyDescent="0.25">
+    <row r="420" spans="18:20" x14ac:dyDescent="0.3">
       <c r="R420">
         <v>0.63609957643160786</v>
       </c>
@@ -26070,7 +26061,7 @@
         <v>2.3247085516717849</v>
       </c>
     </row>
-    <row r="421" spans="18:20" x14ac:dyDescent="0.25">
+    <row r="421" spans="18:20" x14ac:dyDescent="0.3">
       <c r="R421">
         <v>0.64</v>
       </c>
@@ -26081,7 +26072,7 @@
         <v>2.3337916498303573</v>
       </c>
     </row>
-    <row r="422" spans="18:20" x14ac:dyDescent="0.25">
+    <row r="422" spans="18:20" x14ac:dyDescent="0.3">
       <c r="R422">
         <v>0.64390042356839217</v>
       </c>
@@ -26092,7 +26083,7 @@
         <v>2.3428216258112409</v>
       </c>
     </row>
-    <row r="423" spans="18:20" x14ac:dyDescent="0.25">
+    <row r="423" spans="18:20" x14ac:dyDescent="0.3">
       <c r="R423">
         <v>0.64780084713678432</v>
       </c>
@@ -26103,7 +26094,7 @@
         <v>2.351794119792435</v>
       </c>
     </row>
-    <row r="424" spans="18:20" x14ac:dyDescent="0.25">
+    <row r="424" spans="18:20" x14ac:dyDescent="0.3">
       <c r="R424">
         <v>0.65170127070517647</v>
       </c>
@@ -26114,7 +26105,7 @@
         <v>2.3607043746498939</v>
       </c>
     </row>
-    <row r="425" spans="18:20" x14ac:dyDescent="0.25">
+    <row r="425" spans="18:20" x14ac:dyDescent="0.3">
       <c r="R425">
         <v>0.66</v>
       </c>
@@ -26125,7 +26116,7 @@
         <v>2.3792723553353081</v>
       </c>
     </row>
-    <row r="426" spans="18:20" x14ac:dyDescent="0.25">
+    <row r="426" spans="18:20" x14ac:dyDescent="0.3">
       <c r="R426">
         <v>0.66291963193559889</v>
       </c>
@@ -26136,7 +26127,7 @@
         <v>2.3856491618739475</v>
       </c>
     </row>
-    <row r="427" spans="18:20" x14ac:dyDescent="0.25">
+    <row r="427" spans="18:20" x14ac:dyDescent="0.3">
       <c r="R427">
         <v>0.66583926387119774</v>
       </c>
@@ -26147,7 +26138,7 @@
         <v>2.3919340013397918</v>
       </c>
     </row>
-    <row r="428" spans="18:20" x14ac:dyDescent="0.25">
+    <row r="428" spans="18:20" x14ac:dyDescent="0.3">
       <c r="R428">
         <v>0.66875889580679659</v>
       </c>
@@ -26158,7 +26149,7 @@
         <v>2.3981327633635403</v>
       </c>
     </row>
-    <row r="429" spans="18:20" x14ac:dyDescent="0.25">
+    <row r="429" spans="18:20" x14ac:dyDescent="0.3">
       <c r="R429">
         <v>0.67167852774239545</v>
       </c>
@@ -26169,7 +26160,7 @@
         <v>2.4042515707704131</v>
       </c>
     </row>
-    <row r="430" spans="18:20" x14ac:dyDescent="0.25">
+    <row r="430" spans="18:20" x14ac:dyDescent="0.3">
       <c r="R430">
         <v>0.6745981596779943</v>
       </c>
@@ -26180,7 +26171,7 @@
         <v>2.4102944711053049</v>
       </c>
     </row>
-    <row r="431" spans="18:20" x14ac:dyDescent="0.25">
+    <row r="431" spans="18:20" x14ac:dyDescent="0.3">
       <c r="R431">
         <v>0.68</v>
       </c>
@@ -26191,7 +26182,7 @@
         <v>2.421283151709682</v>
       </c>
     </row>
-    <row r="432" spans="18:20" x14ac:dyDescent="0.25">
+    <row r="432" spans="18:20" x14ac:dyDescent="0.3">
       <c r="R432">
         <v>0.6854018403220058</v>
       </c>
@@ -26202,7 +26193,7 @@
         <v>2.4320368382834952</v>
       </c>
     </row>
-    <row r="433" spans="18:20" x14ac:dyDescent="0.25">
+    <row r="433" spans="18:20" x14ac:dyDescent="0.3">
       <c r="R433">
         <v>0.69080368064401154</v>
       </c>
@@ -26213,7 +26204,7 @@
         <v>2.4425696112170412</v>
       </c>
     </row>
-    <row r="434" spans="18:20" x14ac:dyDescent="0.25">
+    <row r="434" spans="18:20" x14ac:dyDescent="0.3">
       <c r="R434">
         <v>0.69620552096601729</v>
       </c>
@@ -26224,7 +26215,7 @@
         <v>2.4528943039133111</v>
       </c>
     </row>
-    <row r="435" spans="18:20" x14ac:dyDescent="0.25">
+    <row r="435" spans="18:20" x14ac:dyDescent="0.3">
       <c r="R435">
         <v>0.70000000000000007</v>
       </c>
@@ -26235,7 +26226,7 @@
         <v>2.4600288268344701</v>
       </c>
     </row>
-    <row r="436" spans="18:20" x14ac:dyDescent="0.25">
+    <row r="436" spans="18:20" x14ac:dyDescent="0.3">
       <c r="R436">
         <v>0.70379447903398284</v>
       </c>
@@ -26246,7 +26237,7 @@
         <v>2.4670701875482703</v>
       </c>
     </row>
-    <row r="437" spans="18:20" x14ac:dyDescent="0.25">
+    <row r="437" spans="18:20" x14ac:dyDescent="0.3">
       <c r="R437">
         <v>0.70758895806796562</v>
       </c>
@@ -26257,7 +26248,7 @@
         <v>2.4740216787987399</v>
       </c>
     </row>
-    <row r="438" spans="18:20" x14ac:dyDescent="0.25">
+    <row r="438" spans="18:20" x14ac:dyDescent="0.3">
       <c r="R438">
         <v>0.7113834371019484</v>
       </c>
@@ -26268,7 +26259,7 @@
         <v>2.480886195959402</v>
       </c>
     </row>
-    <row r="439" spans="18:20" x14ac:dyDescent="0.25">
+    <row r="439" spans="18:20" x14ac:dyDescent="0.3">
       <c r="R439">
         <v>0.71517791613593118</v>
       </c>
@@ -26279,7 +26270,7 @@
         <v>2.4876662172823489</v>
       </c>
     </row>
-    <row r="440" spans="18:20" x14ac:dyDescent="0.25">
+    <row r="440" spans="18:20" x14ac:dyDescent="0.3">
       <c r="R440">
         <v>0.72</v>
       </c>
@@ -26290,7 +26281,7 @@
         <v>2.4961635976991725</v>
       </c>
     </row>
-    <row r="441" spans="18:20" x14ac:dyDescent="0.25">
+    <row r="441" spans="18:20" x14ac:dyDescent="0.3">
       <c r="R441">
         <v>0.72482208386406877</v>
       </c>
@@ -26301,7 +26292,7 @@
         <v>2.5045311252387021</v>
       </c>
     </row>
-    <row r="442" spans="18:20" x14ac:dyDescent="0.25">
+    <row r="442" spans="18:20" x14ac:dyDescent="0.3">
       <c r="R442">
         <v>0.72964416772813756</v>
       </c>
@@ -26312,7 +26303,7 @@
         <v>2.5127711603506557</v>
       </c>
     </row>
-    <row r="443" spans="18:20" x14ac:dyDescent="0.25">
+    <row r="443" spans="18:20" x14ac:dyDescent="0.3">
       <c r="R443">
         <v>0.73446625159220635</v>
       </c>
@@ -26323,7 +26314,7 @@
         <v>2.5208851585902408</v>
       </c>
     </row>
-    <row r="444" spans="18:20" x14ac:dyDescent="0.25">
+    <row r="444" spans="18:20" x14ac:dyDescent="0.3">
       <c r="R444">
         <v>0.73928833545627515</v>
       </c>
@@ -26334,7 +26325,7 @@
         <v>2.5288738143641529</v>
       </c>
     </row>
-    <row r="445" spans="18:20" x14ac:dyDescent="0.25">
+    <row r="445" spans="18:20" x14ac:dyDescent="0.3">
       <c r="R445">
         <v>0.74</v>
       </c>
@@ -26345,7 +26336,7 @@
         <v>2.5300422273761849</v>
       </c>
     </row>
-    <row r="446" spans="18:20" x14ac:dyDescent="0.25">
+    <row r="446" spans="18:20" x14ac:dyDescent="0.3">
       <c r="R446">
         <v>0.74071166454372483</v>
       </c>
@@ -26356,7 +26347,7 @@
         <v>2.5312079056663648</v>
       </c>
     </row>
-    <row r="447" spans="18:20" x14ac:dyDescent="0.25">
+    <row r="447" spans="18:20" x14ac:dyDescent="0.3">
       <c r="R447">
         <v>0.74142332908744968</v>
       </c>
@@ -26367,7 +26358,7 @@
         <v>2.5323708513599175</v>
       </c>
     </row>
-    <row r="448" spans="18:20" x14ac:dyDescent="0.25">
+    <row r="448" spans="18:20" x14ac:dyDescent="0.3">
       <c r="R448">
         <v>0.74213499363117452</v>
       </c>
@@ -26378,7 +26369,7 @@
         <v>2.5335310660139978</v>
       </c>
     </row>
-    <row r="449" spans="18:20" x14ac:dyDescent="0.25">
+    <row r="449" spans="18:20" x14ac:dyDescent="0.3">
       <c r="R449">
         <v>0.74284665817489937</v>
       </c>
@@ -26389,7 +26380,7 @@
         <v>2.5346885490738456</v>
       </c>
     </row>
-    <row r="450" spans="18:20" x14ac:dyDescent="0.25">
+    <row r="450" spans="18:20" x14ac:dyDescent="0.3">
       <c r="R450">
         <v>0.7499633036121478</v>
       </c>
@@ -26400,7 +26391,7 @@
         <v>2.5461123477155967</v>
       </c>
     </row>
-    <row r="451" spans="18:20" x14ac:dyDescent="0.25">
+    <row r="451" spans="18:20" x14ac:dyDescent="0.3">
       <c r="R451">
         <v>0.75707994904939624</v>
       </c>
@@ -26411,7 +26402,7 @@
         <v>2.5572602342832207</v>
       </c>
     </row>
-    <row r="452" spans="18:20" x14ac:dyDescent="0.25">
+    <row r="452" spans="18:20" x14ac:dyDescent="0.3">
       <c r="R452">
         <v>0.76</v>
       </c>
@@ -26422,7 +26413,7 @@
         <v>2.5617541076679098</v>
       </c>
     </row>
-    <row r="453" spans="18:20" x14ac:dyDescent="0.25">
+    <row r="453" spans="18:20" x14ac:dyDescent="0.3">
       <c r="R453">
         <v>0.76292005095060378</v>
       </c>
@@ -26433,7 +26424,7 @@
         <v>2.5662043384136903</v>
       </c>
     </row>
-    <row r="454" spans="18:20" x14ac:dyDescent="0.25">
+    <row r="454" spans="18:20" x14ac:dyDescent="0.3">
       <c r="R454">
         <v>0.76584010190120755</v>
       </c>
@@ -26444,7 +26435,7 @@
         <v>2.5706133886880829</v>
       </c>
     </row>
-    <row r="455" spans="18:20" x14ac:dyDescent="0.25">
+    <row r="455" spans="18:20" x14ac:dyDescent="0.3">
       <c r="R455">
         <v>0.76876015285181132</v>
       </c>
@@ -26455,7 +26446,7 @@
         <v>2.5749814005331322</v>
       </c>
     </row>
-    <row r="456" spans="18:20" x14ac:dyDescent="0.25">
+    <row r="456" spans="18:20" x14ac:dyDescent="0.3">
       <c r="R456">
         <v>0.7775957225864979</v>
       </c>
@@ -26466,7 +26457,7 @@
         <v>2.5878287652839242</v>
       </c>
     </row>
-    <row r="457" spans="18:20" x14ac:dyDescent="0.25">
+    <row r="457" spans="18:20" x14ac:dyDescent="0.3">
       <c r="R457">
         <v>0.78</v>
       </c>
@@ -26477,7 +26468,7 @@
         <v>2.5912840025622272</v>
       </c>
     </row>
-    <row r="458" spans="18:20" x14ac:dyDescent="0.25">
+    <row r="458" spans="18:20" x14ac:dyDescent="0.3">
       <c r="R458">
         <v>0.78240427741350216</v>
       </c>
@@ -26488,7 +26479,7 @@
         <v>2.5947074680291347</v>
       </c>
     </row>
-    <row r="459" spans="18:20" x14ac:dyDescent="0.25">
+    <row r="459" spans="18:20" x14ac:dyDescent="0.3">
       <c r="R459">
         <v>0.78480855482700429</v>
       </c>
@@ -26499,7 +26490,7 @@
         <v>2.5981001780869479</v>
       </c>
     </row>
-    <row r="460" spans="18:20" x14ac:dyDescent="0.25">
+    <row r="460" spans="18:20" x14ac:dyDescent="0.3">
       <c r="R460">
         <v>0.8</v>
       </c>
@@ -26510,7 +26501,7 @@
         <v>2.6185398436412877</v>
       </c>
     </row>
-    <row r="461" spans="18:20" x14ac:dyDescent="0.25">
+    <row r="461" spans="18:20" x14ac:dyDescent="0.3">
       <c r="R461">
         <v>0.80455743355189879</v>
       </c>
@@ -26521,7 +26512,7 @@
         <v>2.6245283256453917</v>
       </c>
     </row>
-    <row r="462" spans="18:20" x14ac:dyDescent="0.25">
+    <row r="462" spans="18:20" x14ac:dyDescent="0.3">
       <c r="R462">
         <v>0.80911486710379754</v>
       </c>
@@ -26532,7 +26523,7 @@
         <v>2.6303945860224776</v>
       </c>
     </row>
-    <row r="463" spans="18:20" x14ac:dyDescent="0.25">
+    <row r="463" spans="18:20" x14ac:dyDescent="0.3">
       <c r="R463">
         <v>0.81367230065569629</v>
       </c>
@@ -26543,7 +26534,7 @@
         <v>2.6361402498224615</v>
       </c>
     </row>
-    <row r="464" spans="18:20" x14ac:dyDescent="0.25">
+    <row r="464" spans="18:20" x14ac:dyDescent="0.3">
       <c r="R464">
         <v>0.82000000000000006</v>
       </c>
@@ -26554,7 +26545,7 @@
         <v>2.6438948632411612</v>
       </c>
     </row>
-    <row r="465" spans="18:20" x14ac:dyDescent="0.25">
+    <row r="465" spans="18:20" x14ac:dyDescent="0.3">
       <c r="R465">
         <v>0.82632769934430383</v>
       </c>
@@ -26565,7 +26556,7 @@
         <v>2.6514153519740224</v>
       </c>
     </row>
-    <row r="466" spans="18:20" x14ac:dyDescent="0.25">
+    <row r="466" spans="18:20" x14ac:dyDescent="0.3">
       <c r="R466">
         <v>0.83265539868860761</v>
       </c>
@@ -26576,7 +26567,7 @@
         <v>2.6586981923574959</v>
       </c>
     </row>
-    <row r="467" spans="18:20" x14ac:dyDescent="0.25">
+    <row r="467" spans="18:20" x14ac:dyDescent="0.3">
       <c r="R467">
         <v>0.83485877908202533</v>
       </c>
@@ -26587,7 +26578,7 @@
         <v>2.6611961554980357</v>
       </c>
     </row>
-    <row r="468" spans="18:20" x14ac:dyDescent="0.25">
+    <row r="468" spans="18:20" x14ac:dyDescent="0.3">
       <c r="R468">
         <v>0.83706215947544305</v>
       </c>
@@ -26598,7 +26589,7 @@
         <v>2.6636629408390897</v>
       </c>
     </row>
-    <row r="469" spans="18:20" x14ac:dyDescent="0.25">
+    <row r="469" spans="18:20" x14ac:dyDescent="0.3">
       <c r="R469">
         <v>0.83926553986886077</v>
       </c>
@@ -26609,7 +26600,7 @@
         <v>2.6661002498773319</v>
       </c>
     </row>
-    <row r="470" spans="18:20" x14ac:dyDescent="0.25">
+    <row r="470" spans="18:20" x14ac:dyDescent="0.3">
       <c r="R470">
         <v>0.84</v>
       </c>
@@ -26620,7 +26611,7 @@
         <v>2.6669084637172293</v>
       </c>
     </row>
-    <row r="471" spans="18:20" x14ac:dyDescent="0.25">
+    <row r="471" spans="18:20" x14ac:dyDescent="0.3">
       <c r="R471">
         <v>0.84073446013113917</v>
       </c>
@@ -26631,7 +26622,7 @@
         <v>2.6677133504833828</v>
       </c>
     </row>
-    <row r="472" spans="18:20" x14ac:dyDescent="0.25">
+    <row r="472" spans="18:20" x14ac:dyDescent="0.3">
       <c r="R472">
         <v>0.84146892026227837</v>
       </c>
@@ -26642,7 +26633,7 @@
         <v>2.6685150380951876</v>
       </c>
     </row>
-    <row r="473" spans="18:20" x14ac:dyDescent="0.25">
+    <row r="473" spans="18:20" x14ac:dyDescent="0.3">
       <c r="R473">
         <v>0.8488135215736704</v>
       </c>
@@ -26653,7 +26644,7 @@
         <v>2.676261056650914</v>
       </c>
     </row>
-    <row r="474" spans="18:20" x14ac:dyDescent="0.25">
+    <row r="474" spans="18:20" x14ac:dyDescent="0.3">
       <c r="R474">
         <v>0.85615812288506243</v>
       </c>
@@ -26664,7 +26655,7 @@
         <v>2.6836925030640968</v>
       </c>
     </row>
-    <row r="475" spans="18:20" x14ac:dyDescent="0.25">
+    <row r="475" spans="18:20" x14ac:dyDescent="0.3">
       <c r="R475">
         <v>0.86</v>
       </c>
@@ -26675,7 +26666,7 @@
         <v>2.6874770952929845</v>
       </c>
     </row>
-    <row r="476" spans="18:20" x14ac:dyDescent="0.25">
+    <row r="476" spans="18:20" x14ac:dyDescent="0.3">
       <c r="R476">
         <v>0.86384187711493754</v>
       </c>
@@ -26686,7 +26677,7 @@
         <v>2.6911681989373815</v>
       </c>
     </row>
-    <row r="477" spans="18:20" x14ac:dyDescent="0.25">
+    <row r="477" spans="18:20" x14ac:dyDescent="0.3">
       <c r="R477">
         <v>0.86768375422987509</v>
       </c>
@@ -26697,7 +26688,7 @@
         <v>2.6947669026698211</v>
       </c>
     </row>
-    <row r="478" spans="18:20" x14ac:dyDescent="0.25">
+    <row r="478" spans="18:20" x14ac:dyDescent="0.3">
       <c r="R478">
         <v>0.88</v>
       </c>
@@ -26708,7 +26699,7 @@
         <v>2.7055139981231768</v>
       </c>
     </row>
-    <row r="479" spans="18:20" x14ac:dyDescent="0.25">
+    <row r="479" spans="18:20" x14ac:dyDescent="0.3">
       <c r="R479">
         <v>0.89231624577012492</v>
       </c>
@@ -26719,7 +26710,7 @@
         <v>2.7153998836680269</v>
       </c>
     </row>
-    <row r="480" spans="18:20" x14ac:dyDescent="0.25">
+    <row r="480" spans="18:20" x14ac:dyDescent="0.3">
       <c r="R480">
         <v>0.9</v>
       </c>
@@ -26730,7 +26721,7 @@
         <v>2.7211849772039725</v>
       </c>
     </row>
-    <row r="481" spans="18:20" x14ac:dyDescent="0.25">
+    <row r="481" spans="18:20" x14ac:dyDescent="0.3">
       <c r="R481">
         <v>0.90768375422987513</v>
       </c>
@@ -26741,7 +26732,7 @@
         <v>2.726609182421651</v>
       </c>
     </row>
-    <row r="482" spans="18:20" x14ac:dyDescent="0.25">
+    <row r="482" spans="18:20" x14ac:dyDescent="0.3">
       <c r="R482">
         <v>0.91536750845975023</v>
       </c>
@@ -26752,7 +26743,7 @@
         <v>2.7316736188386241</v>
       </c>
     </row>
-    <row r="483" spans="18:20" x14ac:dyDescent="0.25">
+    <row r="483" spans="18:20" x14ac:dyDescent="0.3">
       <c r="R483">
         <v>0.92</v>
       </c>
@@ -26763,7 +26754,7 @@
         <v>2.7345798653441769</v>
       </c>
     </row>
-    <row r="484" spans="18:20" x14ac:dyDescent="0.25">
+    <row r="484" spans="18:20" x14ac:dyDescent="0.3">
       <c r="R484">
         <v>0.92463249154024985</v>
       </c>
@@ -26774,7 +26765,7 @@
         <v>2.7373493803380877</v>
       </c>
     </row>
-    <row r="485" spans="18:20" x14ac:dyDescent="0.25">
+    <row r="485" spans="18:20" x14ac:dyDescent="0.3">
       <c r="R485">
         <v>0.92926498308049965</v>
       </c>
@@ -26785,7 +26776,7 @@
         <v>2.7399834348191368</v>
       </c>
     </row>
-    <row r="486" spans="18:20" x14ac:dyDescent="0.25">
+    <row r="486" spans="18:20" x14ac:dyDescent="0.3">
       <c r="R486">
         <v>0.94000000000000006</v>
       </c>
@@ -26796,7 +26787,7 @@
         <v>2.745454733739876</v>
       </c>
     </row>
-    <row r="487" spans="18:20" x14ac:dyDescent="0.25">
+    <row r="487" spans="18:20" x14ac:dyDescent="0.3">
       <c r="R487">
         <v>0.95073501691950046</v>
       </c>
@@ -26807,7 +26798,7 @@
         <v>2.7502460634380328</v>
       </c>
     </row>
-    <row r="488" spans="18:20" x14ac:dyDescent="0.25">
+    <row r="488" spans="18:20" x14ac:dyDescent="0.3">
       <c r="R488">
         <v>0.96</v>
       </c>
@@ -26818,7 +26809,7 @@
         <v>2.7538512468547829</v>
       </c>
     </row>
-    <row r="489" spans="18:20" x14ac:dyDescent="0.25">
+    <row r="489" spans="18:20" x14ac:dyDescent="0.3">
       <c r="R489">
         <v>0.96926498308049946</v>
       </c>
@@ -26829,7 +26820,7 @@
         <v>2.7569332965013231</v>
       </c>
     </row>
-    <row r="490" spans="18:20" x14ac:dyDescent="0.25">
+    <row r="490" spans="18:20" x14ac:dyDescent="0.3">
       <c r="R490">
         <v>0.97852996616099897</v>
       </c>
@@ -26840,7 +26831,7 @@
         <v>2.7594911893336671</v>
       </c>
     </row>
-    <row r="491" spans="18:20" x14ac:dyDescent="0.25">
+    <row r="491" spans="18:20" x14ac:dyDescent="0.3">
       <c r="R491">
         <v>0.98</v>
       </c>
@@ -26851,7 +26842,7 @@
         <v>2.7598643367485285</v>
       </c>
     </row>
-    <row r="492" spans="18:20" x14ac:dyDescent="0.25">
+    <row r="492" spans="18:20" x14ac:dyDescent="0.3">
       <c r="R492">
         <v>0.981470033839001</v>
       </c>
@@ -26862,7 +26853,7 @@
         <v>2.7602315986558992</v>
       </c>
     </row>
-    <row r="493" spans="18:20" x14ac:dyDescent="0.25">
+    <row r="493" spans="18:20" x14ac:dyDescent="0.3">
       <c r="R493">
         <v>0.98294006767800202</v>
       </c>
@@ -26873,7 +26864,7 @@
         <v>2.7605872530826487</v>
       </c>
     </row>
-    <row r="494" spans="18:20" x14ac:dyDescent="0.25">
+    <row r="494" spans="18:20" x14ac:dyDescent="0.3">
       <c r="R494">
         <v>0.98441010151700303</v>
       </c>
@@ -26884,7 +26875,7 @@
         <v>2.7609292141704498</v>
       </c>
     </row>
-    <row r="495" spans="18:20" x14ac:dyDescent="0.25">
+    <row r="495" spans="18:20" x14ac:dyDescent="0.3">
       <c r="R495">
         <v>0.99605791428929691</v>
       </c>
@@ -26895,7 +26886,7 @@
         <v>2.7628979437497279</v>
       </c>
     </row>
-    <row r="496" spans="18:20" x14ac:dyDescent="0.25">
+    <row r="496" spans="18:20" x14ac:dyDescent="0.3">
       <c r="R496">
         <v>0.99999999999999289</v>
       </c>
@@ -26906,7 +26897,7 @@
         <v>2.7634416052061335</v>
       </c>
     </row>
-    <row r="497" spans="18:20" x14ac:dyDescent="0.25">
+    <row r="497" spans="18:20" x14ac:dyDescent="0.3">
       <c r="R497">
         <v>1</v>
       </c>
@@ -26928,16 +26919,16 @@
   <dimension ref="A6:J14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O9" sqref="O9"/>
+      <selection activeCell="J7" sqref="J7:J11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="15.28515625" customWidth="1"/>
+    <col min="2" max="2" width="15.33203125" customWidth="1"/>
     <col min="3" max="3" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B6" t="s">
         <v>19</v>
       </c>
@@ -26956,7 +26947,7 @@
       <c r="G6">
         <v>1000</v>
       </c>
-      <c r="H6" s="6">
+      <c r="H6" s="4">
         <v>1175</v>
       </c>
       <c r="I6">
@@ -26966,7 +26957,7 @@
         <v>1500</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7" s="5" t="s">
         <v>31</v>
       </c>
@@ -26998,7 +26989,7 @@
         <v>11.9</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8" s="5"/>
       <c r="B8" t="s">
         <v>3</v>
@@ -27028,7 +27019,7 @@
         <v>13.1</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A9" s="5"/>
       <c r="B9" t="s">
         <v>4</v>
@@ -27058,7 +27049,7 @@
         <v>7.9</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A10" s="5"/>
       <c r="B10" t="s">
         <v>5</v>
@@ -27088,7 +27079,7 @@
         <v>11.5</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A11" s="5"/>
       <c r="B11" t="s">
         <v>6</v>
@@ -27118,7 +27109,7 @@
         <v>24.6</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B13" t="s">
         <v>35</v>
       </c>
@@ -27127,7 +27118,7 @@
         <v>2.06</v>
       </c>
       <c r="D13">
-        <f t="shared" ref="D13:J13" si="0">AVERAGE(D7:D11)</f>
+        <f t="shared" ref="D13:G13" si="0">AVERAGE(D7:D11)</f>
         <v>3.8</v>
       </c>
       <c r="E13">
@@ -27155,7 +27146,7 @@
         <v>13.8</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B14" t="s">
         <v>36</v>
       </c>
@@ -27164,7 +27155,7 @@
         <v>0.68876701430890253</v>
       </c>
       <c r="D14">
-        <f t="shared" ref="D14:J14" si="1">_xlfn.STDEV.P(D7:D11)</f>
+        <f t="shared" ref="D14:G14" si="1">_xlfn.STDEV.P(D7:D11)</f>
         <v>1.3371611720357421</v>
       </c>
       <c r="E14">

</xml_diff>